<commit_message>
update template excel file
</commit_message>
<xml_diff>
--- a/tm_303_calendar.xlsx
+++ b/tm_303_calendar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="title_block" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
     <sheet name="calendar" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">calendar!$B$2:$O$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">calendar!$B$2:$O$64</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">title_block!$B$2:$O$65</definedName>
     <definedName function="false" hidden="false" name="copy" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="dfdsf" vbProcedure="false">#REF!</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="137">
   <si>
     <r>
       <rPr>
@@ -1794,9 +1794,6 @@
   </si>
   <si>
     <t xml:space="preserve">主题：《立夏》</t>
-  </si>
-  <si>
-    <t xml:space="preserve">林长宏</t>
   </si>
   <si>
     <t xml:space="preserve">会议开场</t>
@@ -2213,7 +2210,7 @@
     <numFmt numFmtId="165" formatCode="H:MM"/>
     <numFmt numFmtId="166" formatCode="H:MM;@"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2417,6 +2414,16 @@
       <name val="宋体"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2803,7 +2810,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="150">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3140,6 +3147,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3284,7 +3303,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3292,11 +3311,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3304,7 +3323,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3312,7 +3331,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3378,6 +3397,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -3471,9 +3494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>270720</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3483,7 +3506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15038640"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3511,9 +3534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>270720</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3523,7 +3546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15038640"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3551,9 +3574,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>294120</xdr:colOff>
+      <xdr:colOff>293040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3567,7 +3590,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="216000" y="273960"/>
-          <a:ext cx="1651320" cy="1343160"/>
+          <a:ext cx="1650240" cy="1342080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3588,9 +3611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>245160</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3600,7 +3623,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="187200" cy="243720"/>
+          <a:ext cx="186120" cy="242640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3628,9 +3651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>245160</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3640,7 +3663,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="187200" cy="243720"/>
+          <a:ext cx="186120" cy="242640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3668,9 +3691,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>245160</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3680,7 +3703,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="187200" cy="243720"/>
+          <a:ext cx="186120" cy="242640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3708,9 +3731,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>245160</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3720,7 +3743,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="187200" cy="243720"/>
+          <a:ext cx="186120" cy="242640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3748,9 +3771,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1315080</xdr:colOff>
+      <xdr:colOff>1314000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3764,7 +3787,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12273120" y="347760"/>
-          <a:ext cx="1060560" cy="1196640"/>
+          <a:ext cx="1059480" cy="1195560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3785,9 +3808,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>196560</xdr:colOff>
+      <xdr:colOff>195480</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3801,7 +3824,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10986840" y="330840"/>
-          <a:ext cx="1228320" cy="1247400"/>
+          <a:ext cx="1227240" cy="1246320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3827,9 +3850,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3839,7 +3862,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3170520"/>
-          <a:ext cx="187200" cy="285120"/>
+          <a:ext cx="186120" cy="284040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3867,9 +3890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3879,7 +3902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3170520"/>
-          <a:ext cx="187200" cy="285120"/>
+          <a:ext cx="186120" cy="284040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3907,9 +3930,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3923,7 +3946,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7699680" y="6546240"/>
-          <a:ext cx="170280" cy="126720"/>
+          <a:ext cx="169200" cy="125640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3944,9 +3967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3956,7 +3979,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3872160"/>
-          <a:ext cx="187200" cy="245880"/>
+          <a:ext cx="186120" cy="244800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3984,9 +4007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3996,7 +4019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3872160"/>
-          <a:ext cx="187200" cy="245880"/>
+          <a:ext cx="186120" cy="244800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4024,9 +4047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4036,7 +4059,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3521160"/>
-          <a:ext cx="187200" cy="284400"/>
+          <a:ext cx="186120" cy="283320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4064,9 +4087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4076,7 +4099,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3521160"/>
-          <a:ext cx="187200" cy="284400"/>
+          <a:ext cx="186120" cy="283320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4104,9 +4127,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4116,7 +4139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3346200"/>
-          <a:ext cx="187200" cy="284040"/>
+          <a:ext cx="186120" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4144,9 +4167,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4156,7 +4179,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3346200"/>
-          <a:ext cx="187200" cy="284040"/>
+          <a:ext cx="186120" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4184,9 +4207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4196,7 +4219,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3696480"/>
-          <a:ext cx="187200" cy="246960"/>
+          <a:ext cx="186120" cy="245880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4224,9 +4247,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4236,7 +4259,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3696480"/>
-          <a:ext cx="187200" cy="246960"/>
+          <a:ext cx="186120" cy="245880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4264,9 +4287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4276,7 +4299,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3521160"/>
-          <a:ext cx="187200" cy="284400"/>
+          <a:ext cx="186120" cy="283320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4304,9 +4327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4316,7 +4339,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6894360" y="3521160"/>
-          <a:ext cx="187200" cy="284400"/>
+          <a:ext cx="186120" cy="283320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4349,9 +4372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>270720</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4360,8 +4383,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894000"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:off x="4789440" y="16084440"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4389,9 +4412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>270720</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4400,8 +4423,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894000"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:off x="4789440" y="16084440"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4423,15 +4446,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>57600</xdr:colOff>
+      <xdr:colOff>58320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>273600</xdr:colOff>
+      <xdr:colOff>273240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4444,8 +4467,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="195120" y="194040"/>
-          <a:ext cx="1651680" cy="1326240"/>
+          <a:off x="195840" y="194760"/>
+          <a:ext cx="1650600" cy="1325160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4466,9 +4489,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4477,8 +4500,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5117400"/>
-          <a:ext cx="187200" cy="414720"/>
+          <a:off x="4789440" y="5307840"/>
+          <a:ext cx="186120" cy="414360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4506,9 +4529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4517,8 +4540,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5117400"/>
-          <a:ext cx="187200" cy="414720"/>
+          <a:off x="4789440" y="5307840"/>
+          <a:ext cx="186120" cy="414360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4546,9 +4569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>266400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>223560</xdr:rowOff>
+      <xdr:rowOff>222480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4561,8 +4584,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5297040" y="11001960"/>
-          <a:ext cx="170280" cy="177840"/>
+          <a:off x="5297040" y="11192400"/>
+          <a:ext cx="169200" cy="176760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4579,13 +4602,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4594,8 +4617,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6375240"/>
-          <a:ext cx="187200" cy="413280"/>
+          <a:off x="4789440" y="6566400"/>
+          <a:ext cx="186120" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4619,13 +4642,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4634,8 +4657,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6375240"/>
-          <a:ext cx="187200" cy="413280"/>
+          <a:off x="4789440" y="6566400"/>
+          <a:ext cx="186120" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4658,14 +4681,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:colOff>291240</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>270360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4674,8 +4697,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16199280"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:off x="4789440" y="16085160"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4698,14 +4721,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:colOff>291240</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>270360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4714,8 +4737,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16199280"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:off x="4789440" y="16085160"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4738,14 +4761,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:colOff>291240</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>270360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4754,8 +4777,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16199280"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:off x="4789440" y="16085160"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4778,14 +4801,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:colOff>291240</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>270360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4794,8 +4817,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16199280"/>
-          <a:ext cx="187200" cy="270720"/>
+          <a:off x="4789440" y="16085160"/>
+          <a:ext cx="186120" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4819,13 +4842,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4834,8 +4857,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5727240"/>
-          <a:ext cx="187200" cy="413640"/>
+          <a:off x="4789440" y="5918400"/>
+          <a:ext cx="186120" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4859,13 +4882,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4874,8 +4897,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5727240"/>
-          <a:ext cx="187200" cy="413640"/>
+          <a:off x="4789440" y="5918400"/>
+          <a:ext cx="186120" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4899,13 +4922,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4914,8 +4937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5422680"/>
-          <a:ext cx="187200" cy="413640"/>
+          <a:off x="4789440" y="5613840"/>
+          <a:ext cx="186120" cy="412560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4939,13 +4962,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4954,8 +4977,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5422680"/>
-          <a:ext cx="187200" cy="413640"/>
+          <a:off x="4789440" y="5613840"/>
+          <a:ext cx="186120" cy="412560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4979,13 +5002,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>254520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>185400</xdr:rowOff>
+      <xdr:rowOff>186120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1315080</xdr:colOff>
+      <xdr:colOff>1314000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4998,8 +5021,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12273120" y="347040"/>
-          <a:ext cx="1060560" cy="1196640"/>
+          <a:off x="12273120" y="347760"/>
+          <a:ext cx="1059480" cy="1195560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5020,9 +5043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5031,8 +5054,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6031800"/>
-          <a:ext cx="187200" cy="414720"/>
+          <a:off x="4789440" y="6222240"/>
+          <a:ext cx="186120" cy="414360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5060,9 +5083,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5071,8 +5094,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6031800"/>
-          <a:ext cx="187200" cy="414720"/>
+          <a:off x="4789440" y="6222240"/>
+          <a:ext cx="186120" cy="414360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5096,13 +5119,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5111,8 +5134,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5727240"/>
-          <a:ext cx="187200" cy="413640"/>
+          <a:off x="4789440" y="5918400"/>
+          <a:ext cx="186120" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5136,13 +5159,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5151,8 +5174,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5727240"/>
-          <a:ext cx="187200" cy="413640"/>
+          <a:off x="4789440" y="5918400"/>
+          <a:ext cx="186120" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5174,15 +5197,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
+      <xdr:colOff>77760</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>196560</xdr:colOff>
+      <xdr:colOff>195480</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5195,8 +5218,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10986120" y="330120"/>
-          <a:ext cx="1229040" cy="1247400"/>
+          <a:off x="10986840" y="330840"/>
+          <a:ext cx="1227240" cy="1246320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5219,7 +5242,7 @@
   <dimension ref="B1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5964,7 +5987,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6162,7 +6185,7 @@
   </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6707,8 +6730,8 @@
   </sheetPr>
   <dimension ref="B2:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6822,7 +6845,7 @@
       <c r="K6" s="3"/>
       <c r="O6" s="10"/>
     </row>
-    <row r="7" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="11" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="20"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6838,7 +6861,7 @@
       </c>
       <c r="O7" s="10"/>
     </row>
-    <row r="8" s="11" customFormat="true" ht="1.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="11" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="20"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -6881,8 +6904,8 @@
       <c r="O9" s="49"/>
     </row>
     <row r="10" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="30" t="n">
-        <v>0.625</v>
+      <c r="B10" s="30" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>15</v>
@@ -6893,11 +6916,11 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
-      <c r="J10" s="32" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="K10" s="33" t="s">
-        <v>86</v>
+      <c r="J10" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="85" t="s">
+        <v>16</v>
       </c>
       <c r="L10" s="50" t="s">
         <v>27</v>
@@ -6917,11 +6940,11 @@
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
-      <c r="J11" s="35" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="K11" s="33" t="s">
-        <v>86</v>
+      <c r="J11" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="85" t="s">
+        <v>18</v>
       </c>
       <c r="L11" s="50"/>
       <c r="M11" s="50"/>
@@ -6933,7 +6956,7 @@
         <v>0.625</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
@@ -6957,7 +6980,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
@@ -6975,7 +6998,7 @@
         <v>0.625694444444444</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L13" s="52" t="s">
         <v>29</v>
@@ -6992,17 +7015,17 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="64"/>
       <c r="D14" s="64"/>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
       <c r="G14" s="64"/>
-      <c r="H14" s="84" t="n">
+      <c r="H14" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="85" t="s">
+      <c r="I14" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="32" t="n">
@@ -7010,7 +7033,7 @@
         <v>0.627083333333333</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L14" s="56" t="s">
         <v>33</v>
@@ -7026,26 +7049,26 @@
       </c>
     </row>
     <row r="15" s="24" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="86" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="87" t="n">
+      <c r="B15" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="90" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="88" t="s">
+      <c r="I15" s="91" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="35" t="n">
         <f aca="false">J14+TIME(0,H15,0)</f>
         <v>0.630555555555556</v>
       </c>
-      <c r="K15" s="89" t="s">
-        <v>92</v>
+      <c r="K15" s="92" t="s">
+        <v>91</v>
       </c>
       <c r="L15" s="59" t="s">
         <v>37</v>
@@ -7061,26 +7084,26 @@
       </c>
     </row>
     <row r="16" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="90" t="n">
+      <c r="B16" s="93" t="n">
         <f aca="false">B12+TIME(0,H12,0)</f>
         <v>0.630555555555556</v>
       </c>
-      <c r="C16" s="91" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="92" t="n">
+      <c r="C16" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="95" t="n">
         <f aca="false">SUM(H17:H21)</f>
         <v>9</v>
       </c>
-      <c r="I16" s="93" t="s">
+      <c r="I16" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="94"/>
-      <c r="K16" s="95"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="98"/>
       <c r="L16" s="62" t="s">
         <v>40</v>
       </c>
@@ -7089,25 +7112,25 @@
       <c r="O16" s="62"/>
     </row>
     <row r="17" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="96" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="97" t="n">
+      <c r="B17" s="99" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="100" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="85" t="s">
+      <c r="I17" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J17" s="32" t="n">
         <f aca="false">B16+TIME(0,H17,0)</f>
         <v>0.632638888888889</v>
       </c>
-      <c r="K17" s="98" t="str">
+      <c r="K17" s="101" t="str">
         <f aca="false">K13</f>
         <v>张合堂</v>
       </c>
@@ -7124,25 +7147,25 @@
     </row>
     <row r="18" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="64"/>
       <c r="D18" s="64"/>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
       <c r="G18" s="64"/>
-      <c r="H18" s="84" t="n">
+      <c r="H18" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="85" t="s">
+      <c r="I18" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J18" s="32" t="n">
         <f aca="false">J17+TIME(0,H18,0)</f>
         <v>0.633333333333333</v>
       </c>
-      <c r="K18" s="99" t="s">
-        <v>96</v>
+      <c r="K18" s="102" t="s">
+        <v>95</v>
       </c>
       <c r="L18" s="64" t="s">
         <v>43</v>
@@ -7157,25 +7180,25 @@
     </row>
     <row r="19" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="64"/>
       <c r="D19" s="64"/>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
       <c r="G19" s="64"/>
-      <c r="H19" s="84" t="n">
+      <c r="H19" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="32" t="n">
         <f aca="false">J18+TIME(0,H19,0)</f>
         <v>0.634027777777778</v>
       </c>
-      <c r="K19" s="100" t="s">
-        <v>98</v>
+      <c r="K19" s="103" t="s">
+        <v>97</v>
       </c>
       <c r="L19" s="64" t="s">
         <v>45</v>
@@ -7189,26 +7212,26 @@
       <c r="O19" s="63"/>
     </row>
     <row r="20" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="101" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="84" t="n">
+      <c r="B20" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="32" t="n">
         <f aca="false">J19+TIME(0,H20,0)</f>
         <v>0.635416666666667</v>
       </c>
-      <c r="K20" s="100" t="s">
-        <v>98</v>
+      <c r="K20" s="103" t="s">
+        <v>97</v>
       </c>
       <c r="L20" s="64" t="s">
         <v>47</v>
@@ -7222,26 +7245,26 @@
       <c r="O20" s="63"/>
     </row>
     <row r="21" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="102" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="84" t="n">
+      <c r="B21" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="I21" s="85" t="s">
+      <c r="I21" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="32" t="n">
         <f aca="false">J20+TIME(0,H21,0)</f>
         <v>0.636805555555555</v>
       </c>
-      <c r="K21" s="103" t="s">
-        <v>101</v>
+      <c r="K21" s="106" t="s">
+        <v>100</v>
       </c>
       <c r="L21" s="64" t="s">
         <v>49</v>
@@ -7255,26 +7278,26 @@
       <c r="O21" s="63"/>
     </row>
     <row r="22" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="102" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="84" t="n">
+      <c r="B22" s="105" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="87" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="85" t="s">
+      <c r="I22" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="32" t="n">
         <f aca="false">J21+TIME(0,H22,0)</f>
         <v>0.640972222222222</v>
       </c>
-      <c r="K22" s="99" t="s">
-        <v>103</v>
+      <c r="K22" s="102" t="s">
+        <v>102</v>
       </c>
       <c r="L22" s="64" t="s">
         <v>51</v>
@@ -7288,26 +7311,26 @@
       <c r="O22" s="63"/>
     </row>
     <row r="23" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="104" t="n">
+      <c r="B23" s="107" t="n">
         <f aca="false">B16+TIME(0,H16,0)</f>
         <v>0.636805555555555</v>
       </c>
-      <c r="C23" s="105" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="106" t="n">
+      <c r="C23" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109" t="n">
         <f aca="false">SUM(H24:H28)</f>
         <v>29</v>
       </c>
-      <c r="I23" s="107" t="s">
+      <c r="I23" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="108"/>
-      <c r="K23" s="108"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="111"/>
       <c r="L23" s="64" t="s">
         <v>53</v>
       </c>
@@ -7320,26 +7343,26 @@
       <c r="O23" s="63"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="109" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="84" t="n">
+      <c r="B24" s="112" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="112"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="85" t="s">
+      <c r="I24" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J24" s="32" t="n">
         <f aca="false">B23+TIME(0,H24,0)</f>
         <v>0.6375</v>
       </c>
-      <c r="K24" s="110" t="s">
-        <v>89</v>
+      <c r="K24" s="113" t="s">
+        <v>88</v>
       </c>
       <c r="L24" s="65" t="s">
         <v>55</v>
@@ -7353,26 +7376,26 @@
       <c r="O24" s="67"/>
     </row>
     <row r="25" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="111" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="112" t="n">
+      <c r="B25" s="114" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="114"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="114"/>
+      <c r="F25" s="114"/>
+      <c r="G25" s="114"/>
+      <c r="H25" s="115" t="n">
         <v>2</v>
       </c>
-      <c r="I25" s="113" t="s">
+      <c r="I25" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="114" t="n">
+      <c r="J25" s="117" t="n">
         <f aca="false">J24+TIME(0,H25,0)</f>
         <v>0.638888888888889</v>
       </c>
-      <c r="K25" s="89" t="s">
-        <v>92</v>
+      <c r="K25" s="92" t="s">
+        <v>91</v>
       </c>
       <c r="L25" s="68" t="s">
         <v>57</v>
@@ -7382,14 +7405,14 @@
       <c r="O25" s="68"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="115" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
+      <c r="B26" s="118" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
       <c r="H26" s="43" t="n">
         <v>18</v>
       </c>
@@ -7400,8 +7423,8 @@
         <f aca="false">J25+TIME(0,H26,0)</f>
         <v>0.651388888888889</v>
       </c>
-      <c r="K26" s="116" t="s">
-        <v>108</v>
+      <c r="K26" s="119" t="s">
+        <v>107</v>
       </c>
       <c r="L26" s="69" t="s">
         <v>58</v>
@@ -7411,26 +7434,26 @@
       <c r="O26" s="69"/>
     </row>
     <row r="27" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="109" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="117" t="n">
+      <c r="B27" s="112" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="120" t="n">
         <v>7</v>
       </c>
-      <c r="I27" s="85" t="s">
+      <c r="I27" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="32" t="n">
         <f aca="false">J26+TIME(0,H27,0)</f>
         <v>0.65625</v>
       </c>
-      <c r="K27" s="103" t="s">
-        <v>110</v>
+      <c r="K27" s="106" t="s">
+        <v>109</v>
       </c>
       <c r="L27" s="69"/>
       <c r="M27" s="69"/>
@@ -7438,25 +7461,25 @@
       <c r="O27" s="69"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="118" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="118"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="119" t="n">
+      <c r="B28" s="121" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="122" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="88" t="s">
+      <c r="I28" s="91" t="s">
         <v>22</v>
       </c>
       <c r="J28" s="35" t="n">
         <f aca="false">J27+TIME(0,H28,0)</f>
         <v>0.656944444444444</v>
       </c>
-      <c r="K28" s="120" t="str">
+      <c r="K28" s="123" t="str">
         <f aca="false">K13</f>
         <v>张合堂</v>
       </c>
@@ -7466,51 +7489,51 @@
       <c r="O28" s="69"/>
     </row>
     <row r="29" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="90" t="n">
+      <c r="B29" s="93" t="n">
         <f aca="false">B23+TIME(0,H23,0)</f>
         <v>0.656944444444444</v>
       </c>
-      <c r="C29" s="91" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="92" t="n">
+      <c r="C29" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="95" t="n">
         <f aca="false">SUM(H30:H36)</f>
         <v>25</v>
       </c>
-      <c r="I29" s="93" t="s">
+      <c r="I29" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="121"/>
-      <c r="K29" s="121"/>
+      <c r="J29" s="124"/>
+      <c r="K29" s="124"/>
       <c r="L29" s="69"/>
       <c r="M29" s="69"/>
       <c r="N29" s="69"/>
       <c r="O29" s="69"/>
     </row>
     <row r="30" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="115" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="115"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
+      <c r="B30" s="118" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="118"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="118"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="118"/>
       <c r="H30" s="43" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="122" t="n">
+      <c r="J30" s="125" t="n">
         <f aca="false">B29+TIME(0,H30,0)</f>
         <v>0.657638888888889</v>
       </c>
-      <c r="K30" s="116" t="str">
+      <c r="K30" s="119" t="str">
         <f aca="false">K13</f>
         <v>张合堂</v>
       </c>
@@ -7520,26 +7543,26 @@
       <c r="O30" s="69"/>
     </row>
     <row r="31" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="101" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="84" t="n">
+      <c r="B31" s="104" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="87" t="n">
         <v>7</v>
       </c>
-      <c r="I31" s="85" t="s">
+      <c r="I31" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J31" s="123" t="n">
+      <c r="J31" s="126" t="n">
         <f aca="false">J30+TIME(0,H31,0)</f>
         <v>0.6625</v>
       </c>
-      <c r="K31" s="103" t="s">
-        <v>113</v>
+      <c r="K31" s="106" t="s">
+        <v>112</v>
       </c>
       <c r="L31" s="69"/>
       <c r="M31" s="69"/>
@@ -7547,25 +7570,25 @@
       <c r="O31" s="69"/>
     </row>
     <row r="32" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="109" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="109"/>
-      <c r="D32" s="109"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="109"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="84" t="n">
+      <c r="B32" s="112" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="112"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="85" t="s">
+      <c r="I32" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="123" t="n">
+      <c r="J32" s="126" t="n">
         <f aca="false">J31+TIME(0,H32,0)</f>
         <v>0.663194444444444</v>
       </c>
-      <c r="K32" s="103" t="str">
+      <c r="K32" s="106" t="str">
         <f aca="false">K30</f>
         <v>张合堂</v>
       </c>
@@ -7575,26 +7598,26 @@
       <c r="O32" s="69"/>
     </row>
     <row r="33" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="109" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="84" t="n">
+      <c r="B33" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="112"/>
+      <c r="G33" s="112"/>
+      <c r="H33" s="87" t="n">
         <v>7</v>
       </c>
-      <c r="I33" s="85" t="s">
+      <c r="I33" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J33" s="123" t="n">
+      <c r="J33" s="126" t="n">
         <f aca="false">J32+TIME(0,H33,0)</f>
         <v>0.668055555555555</v>
       </c>
-      <c r="K33" s="103" t="s">
-        <v>115</v>
+      <c r="K33" s="106" t="s">
+        <v>114</v>
       </c>
       <c r="L33" s="70" t="s">
         <v>59</v>
@@ -7604,25 +7627,25 @@
       <c r="O33" s="70"/>
     </row>
     <row r="34" s="11" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="109" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="84" t="n">
+      <c r="B34" s="112" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="85" t="s">
+      <c r="I34" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="123" t="n">
+      <c r="J34" s="126" t="n">
         <f aca="false">J33+TIME(0,H34,0)</f>
         <v>0.66875</v>
       </c>
-      <c r="K34" s="103" t="str">
+      <c r="K34" s="106" t="str">
         <f aca="false">K13</f>
         <v>张合堂</v>
       </c>
@@ -7634,26 +7657,26 @@
       <c r="O34" s="71"/>
     </row>
     <row r="35" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="101" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="101"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="117" t="n">
+      <c r="B35" s="104" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="120" t="n">
         <v>7</v>
       </c>
-      <c r="I35" s="124" t="s">
+      <c r="I35" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="125" t="n">
+      <c r="J35" s="128" t="n">
         <f aca="false">J34+TIME(0,H35,0)</f>
         <v>0.673611111111111</v>
       </c>
-      <c r="K35" s="126" t="s">
-        <v>117</v>
+      <c r="K35" s="129" t="s">
+        <v>116</v>
       </c>
       <c r="L35" s="71"/>
       <c r="M35" s="71"/>
@@ -7661,25 +7684,25 @@
       <c r="O35" s="71"/>
     </row>
     <row r="36" s="11" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="118" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="118"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="87" t="n">
+      <c r="B36" s="121" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="121"/>
+      <c r="H36" s="90" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="88" t="s">
+      <c r="I36" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="127" t="n">
+      <c r="J36" s="130" t="n">
         <f aca="false">J35+TIME(0,H36,0)</f>
         <v>0.674305555555555</v>
       </c>
-      <c r="K36" s="89" t="str">
+      <c r="K36" s="92" t="str">
         <f aca="false">K30</f>
         <v>张合堂</v>
       </c>
@@ -7689,42 +7712,42 @@
       <c r="O36" s="71"/>
     </row>
     <row r="37" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="90" t="n">
+      <c r="B37" s="93" t="n">
         <f aca="false">B29+TIME(0,H29,0)</f>
         <v>0.674305555555556</v>
       </c>
-      <c r="C37" s="91" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91"/>
-      <c r="F37" s="91"/>
-      <c r="G37" s="91"/>
-      <c r="H37" s="92" t="n">
+      <c r="C37" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="95" t="n">
         <v>5</v>
       </c>
-      <c r="I37" s="93" t="s">
+      <c r="I37" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="94"/>
-      <c r="K37" s="95"/>
+      <c r="J37" s="97"/>
+      <c r="K37" s="98"/>
       <c r="L37" s="71"/>
       <c r="M37" s="71"/>
       <c r="N37" s="71"/>
       <c r="O37" s="71"/>
     </row>
     <row r="38" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="104" t="n">
+      <c r="B38" s="107" t="n">
         <f aca="false">B37+TIME(0,H37,0)</f>
         <v>0.677777777777778</v>
       </c>
-      <c r="C38" s="105" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="105"/>
-      <c r="E38" s="105"/>
-      <c r="F38" s="105"/>
-      <c r="G38" s="105"/>
+      <c r="C38" s="108" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="108"/>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
       <c r="H38" s="38" t="n">
         <f aca="false">SUM(H39:H42)</f>
         <v>10</v>
@@ -7740,25 +7763,25 @@
       <c r="O38" s="71"/>
     </row>
     <row r="39" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="115" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="115"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="115"/>
+      <c r="B39" s="118" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="118"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="118"/>
       <c r="H39" s="43" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="122" t="n">
+      <c r="J39" s="125" t="n">
         <f aca="false">B38+TIME(0,H39,0)</f>
         <v>0.678472222222222</v>
       </c>
-      <c r="K39" s="116" t="str">
+      <c r="K39" s="119" t="str">
         <f aca="false">K13</f>
         <v>张合堂</v>
       </c>
@@ -7768,26 +7791,26 @@
       <c r="O39" s="71"/>
     </row>
     <row r="40" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="101" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
-      <c r="H40" s="84" t="n">
+      <c r="B40" s="104" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="104"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="87" t="n">
         <v>3</v>
       </c>
-      <c r="I40" s="85" t="s">
+      <c r="I40" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J40" s="123" t="n">
+      <c r="J40" s="126" t="n">
         <f aca="false">J39+TIME(0,H40,0)</f>
         <v>0.680555555555556</v>
       </c>
-      <c r="K40" s="103" t="s">
-        <v>101</v>
+      <c r="K40" s="106" t="s">
+        <v>100</v>
       </c>
       <c r="L40" s="71"/>
       <c r="M40" s="71"/>
@@ -7795,26 +7818,26 @@
       <c r="O40" s="71"/>
     </row>
     <row r="41" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="109" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="109"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="109"/>
-      <c r="H41" s="84" t="n">
+      <c r="B41" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="87" t="n">
         <v>3</v>
       </c>
-      <c r="I41" s="85" t="s">
+      <c r="I41" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="123" t="n">
+      <c r="J41" s="126" t="n">
         <f aca="false">J40+TIME(0,H41,0)</f>
         <v>0.682638888888889</v>
       </c>
-      <c r="K41" s="103" t="s">
-        <v>122</v>
+      <c r="K41" s="106" t="s">
+        <v>121</v>
       </c>
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
@@ -7822,26 +7845,26 @@
       <c r="O41" s="71"/>
     </row>
     <row r="42" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="101" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" s="101"/>
-      <c r="D42" s="101"/>
-      <c r="E42" s="101"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="101"/>
-      <c r="H42" s="84" t="n">
+      <c r="B42" s="104" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="104"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="104"/>
+      <c r="F42" s="104"/>
+      <c r="G42" s="104"/>
+      <c r="H42" s="87" t="n">
         <v>3</v>
       </c>
-      <c r="I42" s="85" t="s">
+      <c r="I42" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J42" s="123" t="n">
+      <c r="J42" s="126" t="n">
         <f aca="false">J41+TIME(0,H42,0)</f>
         <v>0.684722222222222</v>
       </c>
-      <c r="K42" s="103" t="s">
-        <v>124</v>
+      <c r="K42" s="106" t="s">
+        <v>123</v>
       </c>
       <c r="L42" s="72" t="s">
         <v>61</v>
@@ -7854,26 +7877,26 @@
       </c>
     </row>
     <row r="43" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="90" t="n">
+      <c r="B43" s="93" t="n">
         <f aca="false">B38+TIME(0,H38,0)</f>
         <v>0.684722222222222</v>
       </c>
-      <c r="C43" s="91" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="92" t="n">
+      <c r="C43" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="94"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="95" t="n">
         <f aca="false">SUM(H44:H48)</f>
         <v>15</v>
       </c>
-      <c r="I43" s="93" t="s">
+      <c r="I43" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="92"/>
-      <c r="K43" s="92"/>
+      <c r="J43" s="95"/>
+      <c r="K43" s="95"/>
       <c r="L43" s="73" t="s">
         <v>62</v>
       </c>
@@ -7885,25 +7908,25 @@
       <c r="P43" s="25"/>
     </row>
     <row r="44" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="128" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="129"/>
-      <c r="D44" s="129"/>
-      <c r="E44" s="129"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="84" t="n">
+      <c r="B44" s="131" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="132"/>
+      <c r="D44" s="132"/>
+      <c r="E44" s="132"/>
+      <c r="F44" s="132"/>
+      <c r="G44" s="133"/>
+      <c r="H44" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="85" t="s">
+      <c r="I44" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J44" s="32" t="n">
         <f aca="false">B43+TIME(0,H44,0)</f>
         <v>0.685416666666667</v>
       </c>
-      <c r="K44" s="99" t="str">
+      <c r="K44" s="102" t="str">
         <f aca="false">K17</f>
         <v>张合堂</v>
       </c>
@@ -7919,24 +7942,24 @@
     </row>
     <row r="45" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="64"/>
       <c r="E45" s="64"/>
       <c r="F45" s="64"/>
       <c r="G45" s="64"/>
-      <c r="H45" s="84" t="n">
+      <c r="H45" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="I45" s="85" t="s">
+      <c r="I45" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J45" s="32" t="n">
         <f aca="false">J44+TIME(0,H45,0)</f>
         <v>0.686805555555556</v>
       </c>
-      <c r="K45" s="99" t="str">
+      <c r="K45" s="102" t="str">
         <f aca="false">K18</f>
         <v>丘愉庄</v>
       </c>
@@ -7951,24 +7974,24 @@
     </row>
     <row r="46" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="64"/>
       <c r="D46" s="64"/>
       <c r="E46" s="64"/>
       <c r="F46" s="64"/>
       <c r="G46" s="64"/>
-      <c r="H46" s="84" t="n">
+      <c r="H46" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="I46" s="85" t="s">
+      <c r="I46" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J46" s="32" t="n">
         <f aca="false">J45+TIME(0,H46,0)</f>
         <v>0.688194444444444</v>
       </c>
-      <c r="K46" s="100" t="str">
+      <c r="K46" s="103" t="str">
         <f aca="false">K19</f>
         <v>xxx</v>
       </c>
@@ -7983,24 +8006,24 @@
     </row>
     <row r="47" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="64"/>
       <c r="D47" s="64"/>
       <c r="E47" s="64"/>
       <c r="F47" s="64"/>
       <c r="G47" s="64"/>
-      <c r="H47" s="84" t="n">
+      <c r="H47" s="87" t="n">
         <v>3</v>
       </c>
-      <c r="I47" s="85" t="s">
+      <c r="I47" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J47" s="32" t="n">
         <f aca="false">J46+TIME(0,H47,0)</f>
         <v>0.690277777777778</v>
       </c>
-      <c r="K47" s="100" t="str">
+      <c r="K47" s="103" t="str">
         <f aca="false">K20</f>
         <v>xxx</v>
       </c>
@@ -8015,25 +8038,25 @@
     </row>
     <row r="48" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="64"/>
       <c r="D48" s="64"/>
       <c r="E48" s="64"/>
       <c r="F48" s="64"/>
       <c r="G48" s="64"/>
-      <c r="H48" s="84" t="n">
+      <c r="H48" s="87" t="n">
         <v>7</v>
       </c>
-      <c r="I48" s="85" t="s">
+      <c r="I48" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J48" s="32" t="n">
         <f aca="false">J47+TIME(0,H48,0)</f>
         <v>0.695138888888889</v>
       </c>
-      <c r="K48" s="103" t="s">
-        <v>101</v>
+      <c r="K48" s="106" t="s">
+        <v>100</v>
       </c>
       <c r="L48" s="76" t="s">
         <v>72</v>
@@ -8044,7 +8067,7 @@
     </row>
     <row r="49" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="47"/>
       <c r="D49" s="47"/>
@@ -8065,26 +8088,26 @@
       <c r="O49" s="81"/>
     </row>
     <row r="50" s="11" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="131" t="n">
+      <c r="B50" s="134" t="n">
         <f aca="false">B43+TIME(0,H43,0)</f>
         <v>0.695138888888889</v>
       </c>
-      <c r="C50" s="132" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="132"/>
-      <c r="E50" s="132"/>
-      <c r="F50" s="132"/>
-      <c r="G50" s="132"/>
-      <c r="H50" s="133" t="n">
+      <c r="C50" s="135" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" s="135"/>
+      <c r="E50" s="135"/>
+      <c r="F50" s="135"/>
+      <c r="G50" s="135"/>
+      <c r="H50" s="136" t="n">
         <f aca="false">SUM(H51:H53)</f>
         <v>8</v>
       </c>
-      <c r="I50" s="134" t="s">
+      <c r="I50" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="135"/>
-      <c r="K50" s="121"/>
+      <c r="J50" s="138"/>
+      <c r="K50" s="124"/>
       <c r="L50" s="73" t="s">
         <v>75</v>
       </c>
@@ -8095,26 +8118,26 @@
       <c r="O50" s="75"/>
     </row>
     <row r="51" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="136" t="s">
-        <v>133</v>
-      </c>
-      <c r="C51" s="137"/>
-      <c r="D51" s="137"/>
-      <c r="E51" s="137"/>
-      <c r="F51" s="137"/>
-      <c r="G51" s="138"/>
-      <c r="H51" s="139" t="n">
+      <c r="B51" s="139" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="140"/>
+      <c r="D51" s="140"/>
+      <c r="E51" s="140"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="141"/>
+      <c r="H51" s="142" t="n">
         <v>4</v>
       </c>
-      <c r="I51" s="140" t="s">
+      <c r="I51" s="143" t="s">
         <v>22</v>
       </c>
-      <c r="J51" s="141" t="n">
+      <c r="J51" s="144" t="n">
         <f aca="false">B50+TIME(0,H51,0)</f>
         <v>0.697916666666667</v>
       </c>
-      <c r="K51" s="103" t="s">
-        <v>89</v>
+      <c r="K51" s="106" t="s">
+        <v>88</v>
       </c>
       <c r="L51" s="76" t="s">
         <v>77</v>
@@ -8126,21 +8149,21 @@
       <c r="O51" s="78"/>
     </row>
     <row r="52" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="142" t="s">
-        <v>134</v>
-      </c>
-      <c r="H52" s="84" t="n">
+      <c r="B52" s="145" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="87" t="n">
         <v>3</v>
       </c>
-      <c r="I52" s="85" t="s">
+      <c r="I52" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="32" t="n">
         <f aca="false">J51+TIME(0,H52,0)</f>
         <v>0.7</v>
       </c>
-      <c r="K52" s="103" t="s">
-        <v>89</v>
+      <c r="K52" s="106" t="s">
+        <v>88</v>
       </c>
       <c r="L52" s="76" t="s">
         <v>79</v>
@@ -8152,26 +8175,26 @@
       <c r="O52" s="78"/>
     </row>
     <row r="53" s="11" customFormat="true" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="128" t="s">
-        <v>135</v>
-      </c>
-      <c r="C53" s="129"/>
-      <c r="D53" s="129"/>
-      <c r="E53" s="129"/>
-      <c r="F53" s="129"/>
-      <c r="G53" s="130"/>
-      <c r="H53" s="84" t="n">
+      <c r="B53" s="131" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="132"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="132"/>
+      <c r="F53" s="132"/>
+      <c r="G53" s="133"/>
+      <c r="H53" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="I53" s="85" t="s">
+      <c r="I53" s="88" t="s">
         <v>22</v>
       </c>
       <c r="J53" s="32" t="n">
         <f aca="false">J52+TIME(0,H53,0)</f>
         <v>0.700694444444444</v>
       </c>
-      <c r="K53" s="103" t="s">
-        <v>136</v>
+      <c r="K53" s="106" t="s">
+        <v>135</v>
       </c>
       <c r="L53" s="76" t="s">
         <v>81</v>
@@ -8181,24 +8204,24 @@
         <v>82</v>
       </c>
       <c r="O53" s="78"/>
-      <c r="P53" s="143"/>
+      <c r="P53" s="146"/>
     </row>
     <row r="54" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="131" t="n">
+      <c r="B54" s="134" t="n">
         <f aca="false">B50+TIME(0,H50,0)</f>
         <v>0.700694444444444</v>
       </c>
-      <c r="C54" s="132" t="s">
-        <v>137</v>
-      </c>
-      <c r="D54" s="132"/>
-      <c r="E54" s="132"/>
-      <c r="F54" s="132"/>
-      <c r="G54" s="132"/>
-      <c r="H54" s="133"/>
-      <c r="I54" s="134"/>
-      <c r="J54" s="144"/>
-      <c r="K54" s="145"/>
+      <c r="C54" s="135" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="135"/>
+      <c r="E54" s="135"/>
+      <c r="F54" s="135"/>
+      <c r="G54" s="135"/>
+      <c r="H54" s="135"/>
+      <c r="I54" s="147"/>
+      <c r="J54" s="148"/>
+      <c r="K54" s="149"/>
       <c r="L54" s="82" t="s">
         <v>83</v>
       </c>
@@ -8207,19 +8230,19 @@
         <v>84</v>
       </c>
       <c r="O54" s="83"/>
-      <c r="P54" s="143"/>
+      <c r="P54" s="146"/>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="79">
@@ -8298,7 +8321,7 @@
     <mergeCell ref="N52:O52"/>
     <mergeCell ref="L53:M53"/>
     <mergeCell ref="N53:O53"/>
-    <mergeCell ref="P53:P56"/>
+    <mergeCell ref="P53:P55"/>
     <mergeCell ref="C54:G54"/>
     <mergeCell ref="L54:M54"/>
     <mergeCell ref="N54:O54"/>

</xml_diff>

<commit_message>
mutual use position config and excel writer
</commit_message>
<xml_diff>
--- a/tm_303_calendar.xlsx
+++ b/tm_303_calendar.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="134">
   <si>
     <r>
       <rPr>
@@ -1796,9 +1796,6 @@
     <t xml:space="preserve">主题：《立夏》</t>
   </si>
   <si>
-    <t xml:space="preserve">会议开场</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="9"/>
@@ -1806,7 +1803,7 @@
         <family val="0"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">主持人开场白</t>
+      <t xml:space="preserve">介绍会议规则以及宾客介绍（限时每位</t>
     </r>
     <r>
       <rPr>
@@ -1815,7 +1812,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(</t>
+      <t xml:space="preserve">30</t>
     </r>
     <r>
       <rPr>
@@ -1824,49 +1821,11 @@
         <family val="0"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">介绍会议主要内容、及可能的议程改动</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
+      <t xml:space="preserve">秒）</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">张合堂</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">介绍会议规则以及宾客介绍（限时每位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">秒）</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">介绍国际演讲会及捷普聚思国际演讲俱乐部</t>
@@ -2178,9 +2137,6 @@
   </si>
   <si>
     <t xml:space="preserve">总体点评师报告</t>
-  </si>
-  <si>
-    <t xml:space="preserve">主持人提示观众投票选出“最佳即兴演讲”“最佳备稿演讲”“最佳点评者”及“最佳会议支持者”，微信小程序投票</t>
   </si>
   <si>
     <t xml:space="preserve">会议尾声</t>
@@ -2210,7 +2166,7 @@
     <numFmt numFmtId="165" formatCode="H:MM"/>
     <numFmt numFmtId="166" formatCode="H:MM;@"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2417,13 +2373,9 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2810,7 +2762,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="148">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3147,16 +3099,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3303,7 +3247,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3311,11 +3255,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3323,7 +3267,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="34" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="33" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3331,7 +3275,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3494,9 +3438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>268920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3506,7 +3450,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15038640"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3534,9 +3478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>268920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3546,7 +3490,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15038640"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3574,9 +3518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>292320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3590,7 +3534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="216000" y="273960"/>
-          <a:ext cx="1650240" cy="1342080"/>
+          <a:ext cx="1649520" cy="1341360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3611,9 +3555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3623,7 +3567,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="186120" cy="242640"/>
+          <a:ext cx="185400" cy="241920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3651,9 +3595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3663,7 +3607,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="186120" cy="242640"/>
+          <a:ext cx="185400" cy="241920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3691,9 +3635,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3703,7 +3647,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="186120" cy="242640"/>
+          <a:ext cx="185400" cy="241920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3731,9 +3675,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3743,7 +3687,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="186120" cy="242640"/>
+          <a:ext cx="185400" cy="241920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3771,9 +3715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1314000</xdr:colOff>
+      <xdr:colOff>1313280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3787,7 +3731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12273120" y="347760"/>
-          <a:ext cx="1059480" cy="1195560"/>
+          <a:ext cx="1058760" cy="1194840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3808,9 +3752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>195480</xdr:colOff>
+      <xdr:colOff>194760</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3824,7 +3768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10986840" y="330840"/>
-          <a:ext cx="1227240" cy="1246320"/>
+          <a:ext cx="1226520" cy="1245600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3844,15 +3788,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3861,8 +3805,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3170520"/>
-          <a:ext cx="186120" cy="284040"/>
+          <a:off x="7316280" y="3170520"/>
+          <a:ext cx="185400" cy="283320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3884,15 +3828,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3901,8 +3845,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3170520"/>
-          <a:ext cx="186120" cy="284040"/>
+          <a:off x="7316280" y="3170520"/>
+          <a:ext cx="185400" cy="283320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3924,15 +3868,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>98280</xdr:colOff>
+      <xdr:colOff>98640</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>46440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3945,8 +3889,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7699680" y="6546240"/>
-          <a:ext cx="169200" cy="125640"/>
+          <a:off x="8121600" y="6546240"/>
+          <a:ext cx="168480" cy="124920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3961,15 +3905,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3978,8 +3922,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3872160"/>
-          <a:ext cx="186120" cy="244800"/>
+          <a:off x="7316280" y="3872520"/>
+          <a:ext cx="185400" cy="244080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4001,15 +3945,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4018,8 +3962,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3872160"/>
-          <a:ext cx="186120" cy="244800"/>
+          <a:off x="7316280" y="3872520"/>
+          <a:ext cx="185400" cy="244080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4041,15 +3985,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4058,8 +4002,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3521160"/>
-          <a:ext cx="186120" cy="283320"/>
+          <a:off x="7316280" y="3521160"/>
+          <a:ext cx="185400" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4081,15 +4025,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4098,8 +4042,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3521160"/>
-          <a:ext cx="186120" cy="283320"/>
+          <a:off x="7316280" y="3521160"/>
+          <a:ext cx="185400" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4121,15 +4065,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4138,8 +4082,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3346200"/>
-          <a:ext cx="186120" cy="282960"/>
+          <a:off x="7316280" y="3346200"/>
+          <a:ext cx="185400" cy="282240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4161,15 +4105,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4178,8 +4122,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3346200"/>
-          <a:ext cx="186120" cy="282960"/>
+          <a:off x="7316280" y="3346200"/>
+          <a:ext cx="185400" cy="282240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4201,15 +4145,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4218,8 +4162,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3696480"/>
-          <a:ext cx="186120" cy="245880"/>
+          <a:off x="7316280" y="3696840"/>
+          <a:ext cx="185400" cy="245160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4241,15 +4185,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4258,8 +4202,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3696480"/>
-          <a:ext cx="186120" cy="245880"/>
+          <a:off x="7316280" y="3696840"/>
+          <a:ext cx="185400" cy="245160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4281,15 +4225,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4298,8 +4242,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3521160"/>
-          <a:ext cx="186120" cy="283320"/>
+          <a:off x="7316280" y="3521160"/>
+          <a:ext cx="185400" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4321,15 +4265,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4338,8 +4282,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6894360" y="3521160"/>
-          <a:ext cx="186120" cy="283320"/>
+          <a:off x="7316280" y="3521160"/>
+          <a:ext cx="185400" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4372,9 +4316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>268920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4384,7 +4328,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="16084440"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4412,9 +4356,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>268920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4424,7 +4368,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="16084440"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4452,9 +4396,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>273240</xdr:colOff>
+      <xdr:colOff>272520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4468,7 +4412,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="195840" y="194760"/>
-          <a:ext cx="1650600" cy="1325160"/>
+          <a:ext cx="1649880" cy="1324440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4489,9 +4433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4501,7 +4445,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5307840"/>
-          <a:ext cx="186120" cy="414360"/>
+          <a:ext cx="185400" cy="413640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4529,9 +4473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4541,7 +4485,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5307840"/>
-          <a:ext cx="186120" cy="414360"/>
+          <a:ext cx="185400" cy="413640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4569,9 +4513,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>266400</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>222480</xdr:rowOff>
+      <xdr:rowOff>221760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4585,7 +4529,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5297040" y="11192400"/>
-          <a:ext cx="169200" cy="176760"/>
+          <a:ext cx="168480" cy="176040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4606,9 +4550,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4618,7 +4562,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="6566400"/>
-          <a:ext cx="186120" cy="411480"/>
+          <a:ext cx="185400" cy="410760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4646,9 +4590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4658,7 +4602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="6566400"/>
-          <a:ext cx="186120" cy="411480"/>
+          <a:ext cx="185400" cy="410760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4686,9 +4630,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>270360</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4698,7 +4642,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="16085160"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4726,9 +4670,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>270360</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4738,7 +4682,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="16085160"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4766,9 +4710,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>270360</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4778,7 +4722,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="16085160"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4806,9 +4750,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>270360</xdr:rowOff>
+      <xdr:rowOff>269640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4818,7 +4762,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="16085160"/>
-          <a:ext cx="186120" cy="269640"/>
+          <a:ext cx="185400" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4846,9 +4790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4858,7 +4802,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5918400"/>
-          <a:ext cx="186120" cy="411840"/>
+          <a:ext cx="185400" cy="411120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4886,9 +4830,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4898,7 +4842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5918400"/>
-          <a:ext cx="186120" cy="411840"/>
+          <a:ext cx="185400" cy="411120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4926,9 +4870,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4938,7 +4882,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5613840"/>
-          <a:ext cx="186120" cy="412560"/>
+          <a:ext cx="185400" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4966,9 +4910,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4978,7 +4922,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5613840"/>
-          <a:ext cx="186120" cy="412560"/>
+          <a:ext cx="185400" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5006,9 +4950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1314000</xdr:colOff>
+      <xdr:colOff>1313280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5022,7 +4966,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12273120" y="347760"/>
-          <a:ext cx="1059480" cy="1195560"/>
+          <a:ext cx="1058760" cy="1194840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5043,9 +4987,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5055,7 +4999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="6222240"/>
-          <a:ext cx="186120" cy="414360"/>
+          <a:ext cx="185400" cy="413640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5083,9 +5027,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5095,7 +5039,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="6222240"/>
-          <a:ext cx="186120" cy="414360"/>
+          <a:ext cx="185400" cy="413640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5123,9 +5067,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5135,7 +5079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5918400"/>
-          <a:ext cx="186120" cy="411840"/>
+          <a:ext cx="185400" cy="411120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5163,9 +5107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5175,7 +5119,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="5918400"/>
-          <a:ext cx="186120" cy="411840"/>
+          <a:ext cx="185400" cy="411120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5203,9 +5147,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>195480</xdr:colOff>
+      <xdr:colOff>194760</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5219,7 +5163,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10986840" y="330840"/>
-          <a:ext cx="1227240" cy="1246320"/>
+          <a:ext cx="1226520" cy="1245600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5242,7 +5186,7 @@
   <dimension ref="B1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C49 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5987,7 +5931,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="C49 J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6078,7 +6022,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="C49 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6086,7 +6030,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.5"/>
   </cols>
   <sheetData>
@@ -6134,7 +6078,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C49 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6186,7 +6130,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C49 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6229,7 +6173,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="C49 K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6335,7 +6279,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C49 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6730,8 +6674,8 @@
   </sheetPr>
   <dimension ref="B2:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6916,10 +6860,10 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
-      <c r="J10" s="84" t="s">
+      <c r="J10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="85" t="s">
+      <c r="K10" s="84" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="50" t="s">
@@ -6940,10 +6884,10 @@
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
-      <c r="J11" s="86" t="s">
+      <c r="J11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="85" t="s">
+      <c r="K11" s="84" t="s">
         <v>18</v>
       </c>
       <c r="L11" s="50"/>
@@ -6952,19 +6896,18 @@
       <c r="O11" s="50"/>
     </row>
     <row r="12" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="36" t="n">
-        <v>0.625</v>
+      <c r="B12" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
-      <c r="H12" s="38" t="n">
-        <f aca="false">SUM(H13:H15)</f>
-        <v>8</v>
+      <c r="H12" s="38" t="s">
+        <v>21</v>
       </c>
       <c r="I12" s="39" t="s">
         <v>22</v>
@@ -6980,25 +6923,24 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="42" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
-      <c r="H13" s="43" t="n">
-        <v>1</v>
+      <c r="H13" s="43" t="s">
+        <v>21</v>
       </c>
       <c r="I13" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="45" t="n">
-        <f aca="false">B12+TIME(0,H13,0)</f>
-        <v>0.625694444444444</v>
+      <c r="J13" s="45" t="s">
+        <v>23</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="L13" s="52" t="s">
         <v>29</v>
@@ -7015,25 +6957,25 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="64" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C14" s="64"/>
       <c r="D14" s="64"/>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
       <c r="G14" s="64"/>
-      <c r="H14" s="87" t="n">
+      <c r="H14" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="88" t="s">
+      <c r="I14" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="32" t="n">
+      <c r="J14" s="32" t="e">
         <f aca="false">J13+TIME(0,H14,0)</f>
-        <v>0.627083333333333</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L14" s="56" t="s">
         <v>33</v>
@@ -7049,26 +6991,26 @@
       </c>
     </row>
     <row r="15" s="24" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="90" t="n">
+      <c r="B15" s="87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="91" t="s">
+      <c r="I15" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="35" t="n">
+      <c r="J15" s="35" t="e">
         <f aca="false">J14+TIME(0,H15,0)</f>
-        <v>0.630555555555556</v>
-      </c>
-      <c r="K15" s="92" t="s">
-        <v>91</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="90" t="s">
+        <v>89</v>
       </c>
       <c r="L15" s="59" t="s">
         <v>37</v>
@@ -7084,26 +7026,26 @@
       </c>
     </row>
     <row r="16" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="93" t="n">
+      <c r="B16" s="91" t="e">
         <f aca="false">B12+TIME(0,H12,0)</f>
-        <v>0.630555555555556</v>
-      </c>
-      <c r="C16" s="94" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="93" t="n">
         <f aca="false">SUM(H17:H21)</f>
         <v>9</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="97"/>
-      <c r="K16" s="98"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="96"/>
       <c r="L16" s="62" t="s">
         <v>40</v>
       </c>
@@ -7112,27 +7054,27 @@
       <c r="O16" s="62"/>
     </row>
     <row r="17" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="99" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="100" t="n">
+      <c r="B17" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="98" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="88" t="s">
+      <c r="I17" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="32" t="n">
+      <c r="J17" s="32" t="e">
         <f aca="false">B16+TIME(0,H17,0)</f>
-        <v>0.632638888888889</v>
-      </c>
-      <c r="K17" s="101" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" s="99" t="str">
         <f aca="false">K13</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L17" s="42" t="s">
         <v>41</v>
@@ -7147,25 +7089,25 @@
     </row>
     <row r="18" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C18" s="64"/>
       <c r="D18" s="64"/>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
       <c r="G18" s="64"/>
-      <c r="H18" s="87" t="n">
+      <c r="H18" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="88" t="s">
+      <c r="I18" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="32" t="n">
+      <c r="J18" s="32" t="e">
         <f aca="false">J17+TIME(0,H18,0)</f>
-        <v>0.633333333333333</v>
-      </c>
-      <c r="K18" s="102" t="s">
-        <v>95</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="100" t="s">
+        <v>93</v>
       </c>
       <c r="L18" s="64" t="s">
         <v>43</v>
@@ -7180,25 +7122,25 @@
     </row>
     <row r="19" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C19" s="64"/>
       <c r="D19" s="64"/>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
       <c r="G19" s="64"/>
-      <c r="H19" s="87" t="n">
+      <c r="H19" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="88" t="s">
+      <c r="I19" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="32" t="n">
+      <c r="J19" s="32" t="e">
         <f aca="false">J18+TIME(0,H19,0)</f>
-        <v>0.634027777777778</v>
-      </c>
-      <c r="K19" s="103" t="s">
-        <v>97</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="101" t="s">
+        <v>95</v>
       </c>
       <c r="L19" s="64" t="s">
         <v>45</v>
@@ -7212,26 +7154,26 @@
       <c r="O19" s="63"/>
     </row>
     <row r="20" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="104" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="87" t="n">
+      <c r="B20" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="I20" s="88" t="s">
+      <c r="I20" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="32" t="n">
+      <c r="J20" s="32" t="e">
         <f aca="false">J19+TIME(0,H20,0)</f>
-        <v>0.635416666666667</v>
-      </c>
-      <c r="K20" s="103" t="s">
-        <v>97</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" s="101" t="s">
+        <v>95</v>
       </c>
       <c r="L20" s="64" t="s">
         <v>47</v>
@@ -7245,26 +7187,26 @@
       <c r="O20" s="63"/>
     </row>
     <row r="21" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="105" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="87" t="n">
+      <c r="B21" s="103" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="I21" s="88" t="s">
+      <c r="I21" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="32" t="n">
+      <c r="J21" s="32" t="e">
         <f aca="false">J20+TIME(0,H21,0)</f>
-        <v>0.636805555555555</v>
-      </c>
-      <c r="K21" s="106" t="s">
-        <v>100</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" s="104" t="s">
+        <v>98</v>
       </c>
       <c r="L21" s="64" t="s">
         <v>49</v>
@@ -7278,26 +7220,26 @@
       <c r="O21" s="63"/>
     </row>
     <row r="22" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="105" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="87" t="n">
+      <c r="B22" s="103" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="85" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="88" t="s">
+      <c r="I22" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="32" t="n">
+      <c r="J22" s="32" t="e">
         <f aca="false">J21+TIME(0,H22,0)</f>
-        <v>0.640972222222222</v>
-      </c>
-      <c r="K22" s="102" t="s">
-        <v>102</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" s="100" t="s">
+        <v>100</v>
       </c>
       <c r="L22" s="64" t="s">
         <v>51</v>
@@ -7311,26 +7253,26 @@
       <c r="O22" s="63"/>
     </row>
     <row r="23" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="107" t="n">
+      <c r="B23" s="105" t="e">
         <f aca="false">B16+TIME(0,H16,0)</f>
-        <v>0.636805555555555</v>
-      </c>
-      <c r="C23" s="108" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="109" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C23" s="106" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="107" t="n">
         <f aca="false">SUM(H24:H28)</f>
         <v>29</v>
       </c>
-      <c r="I23" s="110" t="s">
+      <c r="I23" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="111"/>
-      <c r="K23" s="111"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
       <c r="L23" s="64" t="s">
         <v>53</v>
       </c>
@@ -7343,26 +7285,26 @@
       <c r="O23" s="63"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="112" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="87" t="n">
+      <c r="B24" s="110" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="88" t="s">
+      <c r="I24" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="32" t="n">
+      <c r="J24" s="32" t="e">
         <f aca="false">B23+TIME(0,H24,0)</f>
-        <v>0.6375</v>
-      </c>
-      <c r="K24" s="113" t="s">
-        <v>88</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" s="111" t="s">
+        <v>87</v>
       </c>
       <c r="L24" s="65" t="s">
         <v>55</v>
@@ -7376,26 +7318,26 @@
       <c r="O24" s="67"/>
     </row>
     <row r="25" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="114" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="114"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
-      <c r="G25" s="114"/>
-      <c r="H25" s="115" t="n">
+      <c r="B25" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="112"/>
+      <c r="H25" s="113" t="n">
         <v>2</v>
       </c>
-      <c r="I25" s="116" t="s">
+      <c r="I25" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="117" t="n">
+      <c r="J25" s="115" t="e">
         <f aca="false">J24+TIME(0,H25,0)</f>
-        <v>0.638888888888889</v>
-      </c>
-      <c r="K25" s="92" t="s">
-        <v>91</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" s="90" t="s">
+        <v>89</v>
       </c>
       <c r="L25" s="68" t="s">
         <v>57</v>
@@ -7405,26 +7347,26 @@
       <c r="O25" s="68"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="118" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="118"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
+      <c r="B26" s="116" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="116"/>
       <c r="H26" s="43" t="n">
         <v>18</v>
       </c>
       <c r="I26" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="45" t="n">
+      <c r="J26" s="45" t="e">
         <f aca="false">J25+TIME(0,H26,0)</f>
-        <v>0.651388888888889</v>
-      </c>
-      <c r="K26" s="119" t="s">
-        <v>107</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" s="117" t="s">
+        <v>105</v>
       </c>
       <c r="L26" s="69" t="s">
         <v>58</v>
@@ -7434,26 +7376,26 @@
       <c r="O26" s="69"/>
     </row>
     <row r="27" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="112" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="112"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="112"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="120" t="n">
+      <c r="B27" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="118" t="n">
         <v>7</v>
       </c>
-      <c r="I27" s="88" t="s">
+      <c r="I27" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="32" t="n">
+      <c r="J27" s="32" t="e">
         <f aca="false">J26+TIME(0,H27,0)</f>
-        <v>0.65625</v>
-      </c>
-      <c r="K27" s="106" t="s">
-        <v>109</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="104" t="s">
+        <v>107</v>
       </c>
       <c r="L27" s="69"/>
       <c r="M27" s="69"/>
@@ -7461,27 +7403,27 @@
       <c r="O27" s="69"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="121" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="122" t="n">
+      <c r="B28" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="120" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="91" t="s">
+      <c r="I28" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="J28" s="35" t="n">
+      <c r="J28" s="35" t="e">
         <f aca="false">J27+TIME(0,H28,0)</f>
-        <v>0.656944444444444</v>
-      </c>
-      <c r="K28" s="123" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="121" t="str">
         <f aca="false">K13</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L28" s="69"/>
       <c r="M28" s="69"/>
@@ -7489,53 +7431,53 @@
       <c r="O28" s="69"/>
     </row>
     <row r="29" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="93" t="n">
+      <c r="B29" s="91" t="e">
         <f aca="false">B23+TIME(0,H23,0)</f>
-        <v>0.656944444444444</v>
-      </c>
-      <c r="C29" s="94" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="95" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C29" s="92" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="92"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="93" t="n">
         <f aca="false">SUM(H30:H36)</f>
         <v>25</v>
       </c>
-      <c r="I29" s="96" t="s">
+      <c r="I29" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="124"/>
-      <c r="K29" s="124"/>
+      <c r="J29" s="122"/>
+      <c r="K29" s="122"/>
       <c r="L29" s="69"/>
       <c r="M29" s="69"/>
       <c r="N29" s="69"/>
       <c r="O29" s="69"/>
     </row>
     <row r="30" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="118" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="118"/>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
+      <c r="B30" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="116"/>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="116"/>
       <c r="H30" s="43" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="125" t="n">
+      <c r="J30" s="123" t="e">
         <f aca="false">B29+TIME(0,H30,0)</f>
-        <v>0.657638888888889</v>
-      </c>
-      <c r="K30" s="119" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="117" t="str">
         <f aca="false">K13</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L30" s="69"/>
       <c r="M30" s="69"/>
@@ -7543,26 +7485,26 @@
       <c r="O30" s="69"/>
     </row>
     <row r="31" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="104" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="104"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="104"/>
-      <c r="F31" s="104"/>
-      <c r="G31" s="104"/>
-      <c r="H31" s="87" t="n">
+      <c r="B31" s="102" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="85" t="n">
         <v>7</v>
       </c>
-      <c r="I31" s="88" t="s">
+      <c r="I31" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J31" s="126" t="n">
+      <c r="J31" s="124" t="e">
         <f aca="false">J30+TIME(0,H31,0)</f>
-        <v>0.6625</v>
-      </c>
-      <c r="K31" s="106" t="s">
-        <v>112</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K31" s="104" t="s">
+        <v>110</v>
       </c>
       <c r="L31" s="69"/>
       <c r="M31" s="69"/>
@@ -7570,27 +7512,27 @@
       <c r="O31" s="69"/>
     </row>
     <row r="32" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="112" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="112"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="112"/>
-      <c r="H32" s="87" t="n">
+      <c r="B32" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="110"/>
+      <c r="D32" s="110"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="88" t="s">
+      <c r="I32" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="126" t="n">
+      <c r="J32" s="124" t="e">
         <f aca="false">J31+TIME(0,H32,0)</f>
-        <v>0.663194444444444</v>
-      </c>
-      <c r="K32" s="106" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K32" s="104" t="str">
         <f aca="false">K30</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L32" s="69"/>
       <c r="M32" s="69"/>
@@ -7598,26 +7540,26 @@
       <c r="O32" s="69"/>
     </row>
     <row r="33" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="112" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="87" t="n">
+      <c r="B33" s="110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="110"/>
+      <c r="D33" s="110"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="85" t="n">
         <v>7</v>
       </c>
-      <c r="I33" s="88" t="s">
+      <c r="I33" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J33" s="126" t="n">
+      <c r="J33" s="124" t="e">
         <f aca="false">J32+TIME(0,H33,0)</f>
-        <v>0.668055555555555</v>
-      </c>
-      <c r="K33" s="106" t="s">
-        <v>114</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K33" s="104" t="s">
+        <v>112</v>
       </c>
       <c r="L33" s="70" t="s">
         <v>59</v>
@@ -7627,27 +7569,27 @@
       <c r="O33" s="70"/>
     </row>
     <row r="34" s="11" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="112" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112"/>
-      <c r="H34" s="87" t="n">
+      <c r="B34" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="110"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="88" t="s">
+      <c r="I34" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="126" t="n">
+      <c r="J34" s="124" t="e">
         <f aca="false">J33+TIME(0,H34,0)</f>
-        <v>0.66875</v>
-      </c>
-      <c r="K34" s="106" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K34" s="104" t="str">
         <f aca="false">K13</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L34" s="71" t="s">
         <v>60</v>
@@ -7657,26 +7599,26 @@
       <c r="O34" s="71"/>
     </row>
     <row r="35" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="104" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="120" t="n">
+      <c r="B35" s="102" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="102"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="102"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="118" t="n">
         <v>7</v>
       </c>
-      <c r="I35" s="127" t="s">
+      <c r="I35" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="128" t="n">
+      <c r="J35" s="126" t="e">
         <f aca="false">J34+TIME(0,H35,0)</f>
-        <v>0.673611111111111</v>
-      </c>
-      <c r="K35" s="129" t="s">
-        <v>116</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K35" s="127" t="s">
+        <v>114</v>
       </c>
       <c r="L35" s="71"/>
       <c r="M35" s="71"/>
@@ -7684,27 +7626,27 @@
       <c r="O35" s="71"/>
     </row>
     <row r="36" s="11" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="121" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="121"/>
-      <c r="H36" s="90" t="n">
+      <c r="B36" s="119" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="119"/>
+      <c r="D36" s="119"/>
+      <c r="E36" s="119"/>
+      <c r="F36" s="119"/>
+      <c r="G36" s="119"/>
+      <c r="H36" s="88" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="91" t="s">
+      <c r="I36" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="130" t="n">
+      <c r="J36" s="128" t="e">
         <f aca="false">J35+TIME(0,H36,0)</f>
-        <v>0.674305555555555</v>
-      </c>
-      <c r="K36" s="92" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K36" s="90" t="str">
         <f aca="false">K30</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L36" s="71"/>
       <c r="M36" s="71"/>
@@ -7712,42 +7654,42 @@
       <c r="O36" s="71"/>
     </row>
     <row r="37" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="93" t="n">
+      <c r="B37" s="91" t="e">
         <f aca="false">B29+TIME(0,H29,0)</f>
-        <v>0.674305555555556</v>
-      </c>
-      <c r="C37" s="94" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
-      <c r="F37" s="94"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="95" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C37" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="92"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="92"/>
+      <c r="H37" s="93" t="n">
         <v>5</v>
       </c>
-      <c r="I37" s="96" t="s">
+      <c r="I37" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="97"/>
-      <c r="K37" s="98"/>
+      <c r="J37" s="95"/>
+      <c r="K37" s="96"/>
       <c r="L37" s="71"/>
       <c r="M37" s="71"/>
       <c r="N37" s="71"/>
       <c r="O37" s="71"/>
     </row>
     <row r="38" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="107" t="n">
+      <c r="B38" s="105" t="e">
         <f aca="false">B37+TIME(0,H37,0)</f>
-        <v>0.677777777777778</v>
-      </c>
-      <c r="C38" s="108" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="108"/>
-      <c r="E38" s="108"/>
-      <c r="F38" s="108"/>
-      <c r="G38" s="108"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C38" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
       <c r="H38" s="38" t="n">
         <f aca="false">SUM(H39:H42)</f>
         <v>10</v>
@@ -7763,27 +7705,27 @@
       <c r="O38" s="71"/>
     </row>
     <row r="39" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="118" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="118"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="118"/>
+      <c r="B39" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="116"/>
       <c r="H39" s="43" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="125" t="n">
+      <c r="J39" s="123" t="e">
         <f aca="false">B38+TIME(0,H39,0)</f>
-        <v>0.678472222222222</v>
-      </c>
-      <c r="K39" s="119" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K39" s="117" t="str">
         <f aca="false">K13</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L39" s="71"/>
       <c r="M39" s="71"/>
@@ -7791,26 +7733,26 @@
       <c r="O39" s="71"/>
     </row>
     <row r="40" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="104" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="104"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="104"/>
-      <c r="F40" s="104"/>
-      <c r="G40" s="104"/>
-      <c r="H40" s="87" t="n">
+      <c r="B40" s="102" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="102"/>
+      <c r="H40" s="85" t="n">
         <v>3</v>
       </c>
-      <c r="I40" s="88" t="s">
+      <c r="I40" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J40" s="126" t="n">
+      <c r="J40" s="124" t="e">
         <f aca="false">J39+TIME(0,H40,0)</f>
-        <v>0.680555555555556</v>
-      </c>
-      <c r="K40" s="106" t="s">
-        <v>100</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K40" s="104" t="s">
+        <v>98</v>
       </c>
       <c r="L40" s="71"/>
       <c r="M40" s="71"/>
@@ -7818,26 +7760,26 @@
       <c r="O40" s="71"/>
     </row>
     <row r="41" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="112"/>
-      <c r="H41" s="87" t="n">
+      <c r="B41" s="110" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="110"/>
+      <c r="D41" s="110"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="110"/>
+      <c r="G41" s="110"/>
+      <c r="H41" s="85" t="n">
         <v>3</v>
       </c>
-      <c r="I41" s="88" t="s">
+      <c r="I41" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="126" t="n">
+      <c r="J41" s="124" t="e">
         <f aca="false">J40+TIME(0,H41,0)</f>
-        <v>0.682638888888889</v>
-      </c>
-      <c r="K41" s="106" t="s">
-        <v>121</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K41" s="104" t="s">
+        <v>119</v>
       </c>
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
@@ -7845,26 +7787,26 @@
       <c r="O41" s="71"/>
     </row>
     <row r="42" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="104" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="104"/>
-      <c r="D42" s="104"/>
-      <c r="E42" s="104"/>
-      <c r="F42" s="104"/>
-      <c r="G42" s="104"/>
-      <c r="H42" s="87" t="n">
+      <c r="B42" s="102" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="102"/>
+      <c r="D42" s="102"/>
+      <c r="E42" s="102"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="85" t="n">
         <v>3</v>
       </c>
-      <c r="I42" s="88" t="s">
+      <c r="I42" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J42" s="126" t="n">
+      <c r="J42" s="124" t="e">
         <f aca="false">J41+TIME(0,H42,0)</f>
-        <v>0.684722222222222</v>
-      </c>
-      <c r="K42" s="106" t="s">
-        <v>123</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K42" s="104" t="s">
+        <v>121</v>
       </c>
       <c r="L42" s="72" t="s">
         <v>61</v>
@@ -7877,26 +7819,26 @@
       </c>
     </row>
     <row r="43" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="93" t="n">
+      <c r="B43" s="91" t="e">
         <f aca="false">B38+TIME(0,H38,0)</f>
-        <v>0.684722222222222</v>
-      </c>
-      <c r="C43" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="94"/>
-      <c r="E43" s="94"/>
-      <c r="F43" s="94"/>
-      <c r="G43" s="94"/>
-      <c r="H43" s="95" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C43" s="92" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="92"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="92"/>
+      <c r="H43" s="93" t="n">
         <f aca="false">SUM(H44:H48)</f>
         <v>15</v>
       </c>
-      <c r="I43" s="96" t="s">
+      <c r="I43" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="95"/>
-      <c r="K43" s="95"/>
+      <c r="J43" s="93"/>
+      <c r="K43" s="93"/>
       <c r="L43" s="73" t="s">
         <v>62</v>
       </c>
@@ -7908,27 +7850,27 @@
       <c r="P43" s="25"/>
     </row>
     <row r="44" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="131" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" s="132"/>
-      <c r="D44" s="132"/>
-      <c r="E44" s="132"/>
-      <c r="F44" s="132"/>
-      <c r="G44" s="133"/>
-      <c r="H44" s="87" t="n">
+      <c r="B44" s="129" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="130"/>
+      <c r="D44" s="130"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="130"/>
+      <c r="G44" s="131"/>
+      <c r="H44" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="88" t="s">
+      <c r="I44" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J44" s="32" t="n">
+      <c r="J44" s="32" t="e">
         <f aca="false">B43+TIME(0,H44,0)</f>
-        <v>0.685416666666667</v>
-      </c>
-      <c r="K44" s="102" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K44" s="100" t="str">
         <f aca="false">K17</f>
-        <v>张合堂</v>
+        <v>{host_name}</v>
       </c>
       <c r="L44" s="76" t="s">
         <v>64</v>
@@ -7942,24 +7884,24 @@
     </row>
     <row r="45" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="64"/>
       <c r="E45" s="64"/>
       <c r="F45" s="64"/>
       <c r="G45" s="64"/>
-      <c r="H45" s="87" t="n">
+      <c r="H45" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="I45" s="88" t="s">
+      <c r="I45" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J45" s="32" t="n">
+      <c r="J45" s="32" t="e">
         <f aca="false">J44+TIME(0,H45,0)</f>
-        <v>0.686805555555556</v>
-      </c>
-      <c r="K45" s="102" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K45" s="100" t="str">
         <f aca="false">K18</f>
         <v>丘愉庄</v>
       </c>
@@ -7974,24 +7916,24 @@
     </row>
     <row r="46" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C46" s="64"/>
       <c r="D46" s="64"/>
       <c r="E46" s="64"/>
       <c r="F46" s="64"/>
       <c r="G46" s="64"/>
-      <c r="H46" s="87" t="n">
+      <c r="H46" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="I46" s="88" t="s">
+      <c r="I46" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J46" s="32" t="n">
+      <c r="J46" s="32" t="e">
         <f aca="false">J45+TIME(0,H46,0)</f>
-        <v>0.688194444444444</v>
-      </c>
-      <c r="K46" s="103" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K46" s="101" t="str">
         <f aca="false">K19</f>
         <v>xxx</v>
       </c>
@@ -8006,24 +7948,24 @@
     </row>
     <row r="47" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C47" s="64"/>
       <c r="D47" s="64"/>
       <c r="E47" s="64"/>
       <c r="F47" s="64"/>
       <c r="G47" s="64"/>
-      <c r="H47" s="87" t="n">
+      <c r="H47" s="85" t="n">
         <v>3</v>
       </c>
-      <c r="I47" s="88" t="s">
+      <c r="I47" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J47" s="32" t="n">
+      <c r="J47" s="32" t="e">
         <f aca="false">J46+TIME(0,H47,0)</f>
-        <v>0.690277777777778</v>
-      </c>
-      <c r="K47" s="103" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K47" s="101" t="str">
         <f aca="false">K20</f>
         <v>xxx</v>
       </c>
@@ -8038,25 +7980,25 @@
     </row>
     <row r="48" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C48" s="64"/>
       <c r="D48" s="64"/>
       <c r="E48" s="64"/>
       <c r="F48" s="64"/>
       <c r="G48" s="64"/>
-      <c r="H48" s="87" t="n">
+      <c r="H48" s="85" t="n">
         <v>7</v>
       </c>
-      <c r="I48" s="88" t="s">
+      <c r="I48" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J48" s="32" t="n">
+      <c r="J48" s="32" t="e">
         <f aca="false">J47+TIME(0,H48,0)</f>
-        <v>0.695138888888889</v>
-      </c>
-      <c r="K48" s="106" t="s">
-        <v>100</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K48" s="104" t="s">
+        <v>98</v>
       </c>
       <c r="L48" s="76" t="s">
         <v>72</v>
@@ -8067,9 +8009,11 @@
     </row>
     <row r="49" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" s="47"/>
+        <v>14</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>25</v>
+      </c>
       <c r="D49" s="47"/>
       <c r="E49" s="47"/>
       <c r="F49" s="47"/>
@@ -8088,26 +8032,26 @@
       <c r="O49" s="81"/>
     </row>
     <row r="50" s="11" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="134" t="n">
+      <c r="B50" s="132" t="e">
         <f aca="false">B43+TIME(0,H43,0)</f>
-        <v>0.695138888888889</v>
-      </c>
-      <c r="C50" s="135" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" s="135"/>
-      <c r="E50" s="135"/>
-      <c r="F50" s="135"/>
-      <c r="G50" s="135"/>
-      <c r="H50" s="136" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C50" s="133" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="133"/>
+      <c r="E50" s="133"/>
+      <c r="F50" s="133"/>
+      <c r="G50" s="133"/>
+      <c r="H50" s="134" t="n">
         <f aca="false">SUM(H51:H53)</f>
         <v>8</v>
       </c>
-      <c r="I50" s="137" t="s">
+      <c r="I50" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="138"/>
-      <c r="K50" s="124"/>
+      <c r="J50" s="136"/>
+      <c r="K50" s="122"/>
       <c r="L50" s="73" t="s">
         <v>75</v>
       </c>
@@ -8118,26 +8062,26 @@
       <c r="O50" s="75"/>
     </row>
     <row r="51" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="139" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="140"/>
-      <c r="D51" s="140"/>
-      <c r="E51" s="140"/>
-      <c r="F51" s="140"/>
-      <c r="G51" s="141"/>
-      <c r="H51" s="142" t="n">
+      <c r="B51" s="137" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="138"/>
+      <c r="D51" s="138"/>
+      <c r="E51" s="138"/>
+      <c r="F51" s="138"/>
+      <c r="G51" s="139"/>
+      <c r="H51" s="140" t="n">
         <v>4</v>
       </c>
-      <c r="I51" s="143" t="s">
+      <c r="I51" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="J51" s="144" t="n">
+      <c r="J51" s="142" t="e">
         <f aca="false">B50+TIME(0,H51,0)</f>
-        <v>0.697916666666667</v>
-      </c>
-      <c r="K51" s="106" t="s">
-        <v>88</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K51" s="104" t="s">
+        <v>87</v>
       </c>
       <c r="L51" s="76" t="s">
         <v>77</v>
@@ -8149,21 +8093,21 @@
       <c r="O51" s="78"/>
     </row>
     <row r="52" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="145" t="s">
-        <v>133</v>
-      </c>
-      <c r="H52" s="87" t="n">
+      <c r="B52" s="143" t="s">
+        <v>130</v>
+      </c>
+      <c r="H52" s="85" t="n">
         <v>3</v>
       </c>
-      <c r="I52" s="88" t="s">
+      <c r="I52" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J52" s="32" t="n">
+      <c r="J52" s="32" t="e">
         <f aca="false">J51+TIME(0,H52,0)</f>
-        <v>0.7</v>
-      </c>
-      <c r="K52" s="106" t="s">
-        <v>88</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K52" s="104" t="s">
+        <v>87</v>
       </c>
       <c r="L52" s="76" t="s">
         <v>79</v>
@@ -8175,26 +8119,26 @@
       <c r="O52" s="78"/>
     </row>
     <row r="53" s="11" customFormat="true" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="131" t="s">
-        <v>134</v>
-      </c>
-      <c r="C53" s="132"/>
-      <c r="D53" s="132"/>
-      <c r="E53" s="132"/>
-      <c r="F53" s="132"/>
-      <c r="G53" s="133"/>
-      <c r="H53" s="87" t="n">
+      <c r="B53" s="129" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="130"/>
+      <c r="D53" s="130"/>
+      <c r="E53" s="130"/>
+      <c r="F53" s="130"/>
+      <c r="G53" s="131"/>
+      <c r="H53" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="I53" s="88" t="s">
+      <c r="I53" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="J53" s="32" t="n">
+      <c r="J53" s="32" t="e">
         <f aca="false">J52+TIME(0,H53,0)</f>
-        <v>0.700694444444444</v>
-      </c>
-      <c r="K53" s="106" t="s">
-        <v>135</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K53" s="104" t="s">
+        <v>132</v>
       </c>
       <c r="L53" s="76" t="s">
         <v>81</v>
@@ -8204,24 +8148,24 @@
         <v>82</v>
       </c>
       <c r="O53" s="78"/>
-      <c r="P53" s="146"/>
+      <c r="P53" s="144"/>
     </row>
     <row r="54" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="134" t="n">
+      <c r="B54" s="132" t="e">
         <f aca="false">B50+TIME(0,H50,0)</f>
-        <v>0.700694444444444</v>
-      </c>
-      <c r="C54" s="135" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" s="135"/>
-      <c r="E54" s="135"/>
-      <c r="F54" s="135"/>
-      <c r="G54" s="135"/>
-      <c r="H54" s="135"/>
-      <c r="I54" s="147"/>
-      <c r="J54" s="148"/>
-      <c r="K54" s="149"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C54" s="133" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="133"/>
+      <c r="E54" s="133"/>
+      <c r="F54" s="133"/>
+      <c r="G54" s="133"/>
+      <c r="H54" s="133"/>
+      <c r="I54" s="145"/>
+      <c r="J54" s="146"/>
+      <c r="K54" s="147"/>
       <c r="L54" s="82" t="s">
         <v>83</v>
       </c>
@@ -8230,7 +8174,7 @@
         <v>84</v>
       </c>
       <c r="O54" s="83"/>
-      <c r="P54" s="146"/>
+      <c r="P54" s="144"/>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
write data for title and theme block
</commit_message>
<xml_diff>
--- a/tm_303_calendar.xlsx
+++ b/tm_303_calendar.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -1793,7 +1793,106 @@
     <t xml:space="preserve">5. 专业展示 Demonstrating Expertise</t>
   </si>
   <si>
-    <t xml:space="preserve">主题：《立夏》</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="24"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="24"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">会议标题</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="24"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">日期</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">线上：</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">线上会议号</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">摄影师：{摄影师}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">主题：{主题}</t>
   </si>
   <si>
     <r>
@@ -2166,7 +2265,7 @@
     <numFmt numFmtId="165" formatCode="H:MM"/>
     <numFmt numFmtId="166" formatCode="H:MM;@"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2368,6 +2467,13 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="宋体"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
     </font>
@@ -2762,7 +2868,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3099,7 +3205,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3247,7 +3357,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3255,11 +3365,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3267,7 +3377,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="33" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3275,7 +3385,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3438,9 +3548,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>268920</xdr:rowOff>
+      <xdr:rowOff>268560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3450,7 +3560,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15038640"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3478,9 +3588,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>268920</xdr:rowOff>
+      <xdr:rowOff>268560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3490,7 +3600,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15038640"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3518,9 +3628,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3534,7 +3644,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="216000" y="273960"/>
-          <a:ext cx="1649520" cy="1341360"/>
+          <a:ext cx="1649160" cy="1341000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3555,9 +3665,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>243360</xdr:rowOff>
+      <xdr:rowOff>243000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3567,7 +3677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="185400" cy="241920"/>
+          <a:ext cx="185040" cy="241560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3595,9 +3705,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>243360</xdr:rowOff>
+      <xdr:rowOff>243000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3607,7 +3717,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="185400" cy="241920"/>
+          <a:ext cx="185040" cy="241560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3635,9 +3745,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>243360</xdr:rowOff>
+      <xdr:rowOff>243000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3647,7 +3757,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="185400" cy="241920"/>
+          <a:ext cx="185040" cy="241560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3675,9 +3785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>243360</xdr:rowOff>
+      <xdr:rowOff>243000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3687,7 +3797,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789440" y="15344640"/>
-          <a:ext cx="185400" cy="241920"/>
+          <a:ext cx="185040" cy="241560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3715,9 +3825,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1313280</xdr:colOff>
+      <xdr:colOff>1312920</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>102600</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3731,7 +3841,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12273120" y="347760"/>
-          <a:ext cx="1058760" cy="1194840"/>
+          <a:ext cx="1058400" cy="1194480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3752,9 +3862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>194760</xdr:colOff>
+      <xdr:colOff>194400</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3768,7 +3878,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10986840" y="330840"/>
-          <a:ext cx="1226520" cy="1245600"/>
+          <a:ext cx="1226160" cy="1245240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3794,9 +3904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3806,7 +3916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3170520"/>
-          <a:ext cx="185400" cy="283320"/>
+          <a:ext cx="185040" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3834,9 +3944,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3846,7 +3956,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3170520"/>
-          <a:ext cx="185400" cy="283320"/>
+          <a:ext cx="185040" cy="282960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3874,9 +3984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3890,7 +4000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8121600" y="6546240"/>
-          <a:ext cx="168480" cy="124920"/>
+          <a:ext cx="168120" cy="124560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3911,9 +4021,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3923,7 +4033,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3872520"/>
-          <a:ext cx="185400" cy="244080"/>
+          <a:ext cx="185040" cy="243720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3951,9 +4061,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3963,7 +4073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3872520"/>
-          <a:ext cx="185400" cy="244080"/>
+          <a:ext cx="185040" cy="243720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3991,9 +4101,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4003,7 +4113,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3521160"/>
-          <a:ext cx="185400" cy="282960"/>
+          <a:ext cx="185040" cy="282600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4031,9 +4141,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4043,7 +4153,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3521160"/>
-          <a:ext cx="185400" cy="282960"/>
+          <a:ext cx="185040" cy="282600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4071,9 +4181,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4083,7 +4193,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3346200"/>
-          <a:ext cx="185400" cy="282240"/>
+          <a:ext cx="185040" cy="281880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4111,9 +4221,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4123,7 +4233,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3346200"/>
-          <a:ext cx="185400" cy="282240"/>
+          <a:ext cx="185040" cy="281880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4151,9 +4261,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4163,7 +4273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3696840"/>
-          <a:ext cx="185400" cy="245160"/>
+          <a:ext cx="185040" cy="244800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4191,9 +4301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4203,7 +4313,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3696840"/>
-          <a:ext cx="185400" cy="245160"/>
+          <a:ext cx="185040" cy="244800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4231,9 +4341,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4243,7 +4353,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3521160"/>
-          <a:ext cx="185400" cy="282960"/>
+          <a:ext cx="185040" cy="282600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4271,9 +4381,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>291600</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4283,7 +4393,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7316280" y="3521160"/>
-          <a:ext cx="185400" cy="282960"/>
+          <a:ext cx="185040" cy="282600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4316,9 +4426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>268920</xdr:rowOff>
+      <xdr:rowOff>268560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4327,8 +4437,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16084440"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:off x="4789440" y="16011360"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4356,9 +4466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>268920</xdr:rowOff>
+      <xdr:rowOff>268560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4367,8 +4477,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16084440"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:off x="4789440" y="16011360"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4390,9 +4500,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:colOff>58680</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -4411,8 +4521,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="195840" y="194760"/>
-          <a:ext cx="1649880" cy="1324440"/>
+          <a:off x="196200" y="195120"/>
+          <a:ext cx="1649520" cy="1251000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4429,13 +4539,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4444,8 +4554,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5307840"/>
-          <a:ext cx="185400" cy="413640"/>
+          <a:off x="4789440" y="5235120"/>
+          <a:ext cx="185040" cy="412920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4469,13 +4579,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4484,8 +4594,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5307840"/>
-          <a:ext cx="185400" cy="413640"/>
+          <a:off x="4789440" y="5235120"/>
+          <a:ext cx="185040" cy="412920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4513,9 +4623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>265680</xdr:colOff>
+      <xdr:colOff>265320</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>221760</xdr:rowOff>
+      <xdr:rowOff>221400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4528,8 +4638,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5297040" y="11192400"/>
-          <a:ext cx="168480" cy="176040"/>
+          <a:off x="5297040" y="11119320"/>
+          <a:ext cx="168120" cy="175680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4550,7 +4660,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
@@ -4561,8 +4671,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6566400"/>
-          <a:ext cx="185400" cy="410760"/>
+          <a:off x="4789440" y="6493680"/>
+          <a:ext cx="185040" cy="410400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4590,7 +4700,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
@@ -4601,8 +4711,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6566400"/>
-          <a:ext cx="185400" cy="410760"/>
+          <a:off x="4789440" y="6493680"/>
+          <a:ext cx="185040" cy="410400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4630,9 +4740,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>269280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4641,8 +4751,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16085160"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:off x="4789440" y="16012080"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4670,9 +4780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>269280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4681,8 +4791,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16085160"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:off x="4789440" y="16012080"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4710,9 +4820,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>269280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4721,8 +4831,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16085160"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:off x="4789440" y="16012080"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4750,9 +4860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>269280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4761,8 +4871,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="16085160"/>
-          <a:ext cx="185400" cy="268920"/>
+          <a:off x="4789440" y="16012080"/>
+          <a:ext cx="185040" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4786,11 +4896,11 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
@@ -4801,8 +4911,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5918400"/>
-          <a:ext cx="185400" cy="411120"/>
+          <a:off x="4789440" y="5845680"/>
+          <a:ext cx="185040" cy="410760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4826,11 +4936,11 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
@@ -4841,8 +4951,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5918400"/>
-          <a:ext cx="185400" cy="411120"/>
+          <a:off x="4789440" y="5845680"/>
+          <a:ext cx="185040" cy="410760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4870,7 +4980,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
@@ -4881,8 +4991,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5613840"/>
-          <a:ext cx="185400" cy="411840"/>
+          <a:off x="4789440" y="5540760"/>
+          <a:ext cx="185040" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4910,7 +5020,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
@@ -4921,8 +5031,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5613840"/>
-          <a:ext cx="185400" cy="411840"/>
+          <a:off x="4789440" y="5540760"/>
+          <a:ext cx="185040" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4946,11 +5056,11 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>254520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>186120</xdr:rowOff>
+      <xdr:rowOff>186480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1313280</xdr:colOff>
+      <xdr:colOff>1312920</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
@@ -4965,8 +5075,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12273120" y="347760"/>
-          <a:ext cx="1058760" cy="1194840"/>
+          <a:off x="12273120" y="348120"/>
+          <a:ext cx="1058400" cy="1121400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4983,13 +5093,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4998,8 +5108,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6222240"/>
-          <a:ext cx="185400" cy="413640"/>
+          <a:off x="4789440" y="6149520"/>
+          <a:ext cx="185040" cy="413280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5023,13 +5133,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5038,8 +5148,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6222240"/>
-          <a:ext cx="185400" cy="413640"/>
+          <a:off x="4789440" y="6149520"/>
+          <a:ext cx="185040" cy="413280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5063,11 +5173,11 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
@@ -5078,8 +5188,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5918400"/>
-          <a:ext cx="185400" cy="411120"/>
+          <a:off x="4789440" y="5845680"/>
+          <a:ext cx="185040" cy="410760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5103,11 +5213,11 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>290520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
@@ -5118,8 +5228,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5918400"/>
-          <a:ext cx="185400" cy="411120"/>
+          <a:off x="4789440" y="5845680"/>
+          <a:ext cx="185040" cy="410760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5141,13 +5251,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>77760</xdr:colOff>
+      <xdr:colOff>78120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>194760</xdr:colOff>
+      <xdr:colOff>194400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
@@ -5162,8 +5272,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10986840" y="330840"/>
-          <a:ext cx="1226520" cy="1245600"/>
+          <a:off x="10987200" y="331200"/>
+          <a:ext cx="1225800" cy="1172160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5186,7 +5296,7 @@
   <dimension ref="B1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C49 B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5931,7 +6041,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="C49 J3"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6022,7 +6132,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="C49 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6078,7 +6188,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C49 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6130,7 +6240,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C49 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6173,7 +6283,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="C49 K3"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6279,7 +6389,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C49 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6674,8 +6784,8 @@
   </sheetPr>
   <dimension ref="B2:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6716,22 +6826,22 @@
       <c r="N2" s="6"/>
       <c r="O2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="36.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
+      <c r="E3" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
       <c r="O3" s="10"/>
     </row>
     <row r="4" s="11" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6760,7 +6870,7 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="16" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
@@ -6775,13 +6885,13 @@
     </row>
     <row r="6" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="18" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="19" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
@@ -6801,7 +6911,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="M7" s="21" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="O7" s="10"/>
     </row>
@@ -6826,7 +6936,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -6863,7 +6973,7 @@
       <c r="J10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="85" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="50" t="s">
@@ -6887,7 +6997,7 @@
       <c r="J11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="85" t="s">
         <v>18</v>
       </c>
       <c r="L11" s="50"/>
@@ -6957,17 +7067,17 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="64" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C14" s="64"/>
       <c r="D14" s="64"/>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
       <c r="G14" s="64"/>
-      <c r="H14" s="85" t="n">
+      <c r="H14" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="86" t="s">
+      <c r="I14" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="32" t="e">
@@ -6975,7 +7085,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L14" s="56" t="s">
         <v>33</v>
@@ -6991,26 +7101,26 @@
       </c>
     </row>
     <row r="15" s="24" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="88" t="n">
+      <c r="B15" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="89" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="89" t="s">
+      <c r="I15" s="90" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="35" t="e">
         <f aca="false">J14+TIME(0,H15,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K15" s="90" t="s">
-        <v>89</v>
+      <c r="K15" s="91" t="s">
+        <v>94</v>
       </c>
       <c r="L15" s="59" t="s">
         <v>37</v>
@@ -7026,26 +7136,26 @@
       </c>
     </row>
     <row r="16" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="91" t="e">
+      <c r="B16" s="92" t="e">
         <f aca="false">B12+TIME(0,H12,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C16" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="93" t="n">
+      <c r="C16" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="94" t="n">
         <f aca="false">SUM(H17:H21)</f>
         <v>9</v>
       </c>
-      <c r="I16" s="94" t="s">
+      <c r="I16" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="95"/>
-      <c r="K16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="97"/>
       <c r="L16" s="62" t="s">
         <v>40</v>
       </c>
@@ -7054,25 +7164,25 @@
       <c r="O16" s="62"/>
     </row>
     <row r="17" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="97" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="97"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="98" t="n">
+      <c r="B17" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="99" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="86" t="s">
+      <c r="I17" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J17" s="32" t="e">
         <f aca="false">B16+TIME(0,H17,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K17" s="99" t="str">
+      <c r="K17" s="100" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
@@ -7089,25 +7199,25 @@
     </row>
     <row r="18" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="64" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C18" s="64"/>
       <c r="D18" s="64"/>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
       <c r="G18" s="64"/>
-      <c r="H18" s="85" t="n">
+      <c r="H18" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="86" t="s">
+      <c r="I18" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J18" s="32" t="e">
         <f aca="false">J17+TIME(0,H18,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K18" s="100" t="s">
-        <v>93</v>
+      <c r="K18" s="101" t="s">
+        <v>98</v>
       </c>
       <c r="L18" s="64" t="s">
         <v>43</v>
@@ -7122,25 +7232,25 @@
     </row>
     <row r="19" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="64" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C19" s="64"/>
       <c r="D19" s="64"/>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
       <c r="G19" s="64"/>
-      <c r="H19" s="85" t="n">
+      <c r="H19" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="86" t="s">
+      <c r="I19" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="32" t="e">
         <f aca="false">J18+TIME(0,H19,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K19" s="101" t="s">
-        <v>95</v>
+      <c r="K19" s="102" t="s">
+        <v>100</v>
       </c>
       <c r="L19" s="64" t="s">
         <v>45</v>
@@ -7154,26 +7264,26 @@
       <c r="O19" s="63"/>
     </row>
     <row r="20" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="102" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="102"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="85" t="n">
+      <c r="B20" s="103" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="I20" s="86" t="s">
+      <c r="I20" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="32" t="e">
         <f aca="false">J19+TIME(0,H20,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K20" s="101" t="s">
-        <v>95</v>
+      <c r="K20" s="102" t="s">
+        <v>100</v>
       </c>
       <c r="L20" s="64" t="s">
         <v>47</v>
@@ -7187,26 +7297,26 @@
       <c r="O20" s="63"/>
     </row>
     <row r="21" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="103" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="103"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="85" t="n">
+      <c r="B21" s="104" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="I21" s="86" t="s">
+      <c r="I21" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="32" t="e">
         <f aca="false">J20+TIME(0,H21,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K21" s="104" t="s">
-        <v>98</v>
+      <c r="K21" s="105" t="s">
+        <v>103</v>
       </c>
       <c r="L21" s="64" t="s">
         <v>49</v>
@@ -7220,26 +7330,26 @@
       <c r="O21" s="63"/>
     </row>
     <row r="22" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="103" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="85" t="n">
+      <c r="B22" s="104" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="86" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="86" t="s">
+      <c r="I22" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="32" t="e">
         <f aca="false">J21+TIME(0,H22,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K22" s="100" t="s">
-        <v>100</v>
+      <c r="K22" s="101" t="s">
+        <v>105</v>
       </c>
       <c r="L22" s="64" t="s">
         <v>51</v>
@@ -7253,26 +7363,26 @@
       <c r="O22" s="63"/>
     </row>
     <row r="23" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="105" t="e">
+      <c r="B23" s="106" t="e">
         <f aca="false">B16+TIME(0,H16,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C23" s="106" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="106"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="107" t="n">
+      <c r="C23" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="108" t="n">
         <f aca="false">SUM(H24:H28)</f>
         <v>29</v>
       </c>
-      <c r="I23" s="108" t="s">
+      <c r="I23" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
+      <c r="J23" s="110"/>
+      <c r="K23" s="110"/>
       <c r="L23" s="64" t="s">
         <v>53</v>
       </c>
@@ -7285,26 +7395,26 @@
       <c r="O23" s="63"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="110" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="85" t="n">
+      <c r="B24" s="111" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="86" t="s">
+      <c r="I24" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J24" s="32" t="e">
         <f aca="false">B23+TIME(0,H24,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K24" s="111" t="s">
-        <v>87</v>
+      <c r="K24" s="112" t="s">
+        <v>92</v>
       </c>
       <c r="L24" s="65" t="s">
         <v>55</v>
@@ -7318,26 +7428,26 @@
       <c r="O24" s="67"/>
     </row>
     <row r="25" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="112" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="113" t="n">
+      <c r="B25" s="113" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="114" t="n">
         <v>2</v>
       </c>
-      <c r="I25" s="114" t="s">
+      <c r="I25" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="115" t="e">
+      <c r="J25" s="116" t="e">
         <f aca="false">J24+TIME(0,H25,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K25" s="90" t="s">
-        <v>89</v>
+      <c r="K25" s="91" t="s">
+        <v>94</v>
       </c>
       <c r="L25" s="68" t="s">
         <v>57</v>
@@ -7347,14 +7457,14 @@
       <c r="O25" s="68"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="116" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
+      <c r="B26" s="117" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
       <c r="H26" s="43" t="n">
         <v>18</v>
       </c>
@@ -7365,8 +7475,8 @@
         <f aca="false">J25+TIME(0,H26,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K26" s="117" t="s">
-        <v>105</v>
+      <c r="K26" s="118" t="s">
+        <v>110</v>
       </c>
       <c r="L26" s="69" t="s">
         <v>58</v>
@@ -7376,26 +7486,26 @@
       <c r="O26" s="69"/>
     </row>
     <row r="27" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="110" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="118" t="n">
+      <c r="B27" s="111" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="119" t="n">
         <v>7</v>
       </c>
-      <c r="I27" s="86" t="s">
+      <c r="I27" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="32" t="e">
         <f aca="false">J26+TIME(0,H27,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K27" s="104" t="s">
-        <v>107</v>
+      <c r="K27" s="105" t="s">
+        <v>112</v>
       </c>
       <c r="L27" s="69"/>
       <c r="M27" s="69"/>
@@ -7403,25 +7513,25 @@
       <c r="O27" s="69"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="119" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="119"/>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="120" t="n">
+      <c r="B28" s="120" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="120"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="120"/>
+      <c r="F28" s="120"/>
+      <c r="G28" s="120"/>
+      <c r="H28" s="121" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="89" t="s">
+      <c r="I28" s="90" t="s">
         <v>22</v>
       </c>
       <c r="J28" s="35" t="e">
         <f aca="false">J27+TIME(0,H28,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K28" s="121" t="str">
+      <c r="K28" s="122" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
@@ -7431,51 +7541,51 @@
       <c r="O28" s="69"/>
     </row>
     <row r="29" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="91" t="e">
+      <c r="B29" s="92" t="e">
         <f aca="false">B23+TIME(0,H23,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C29" s="92" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="93" t="n">
+      <c r="C29" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="93"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="94" t="n">
         <f aca="false">SUM(H30:H36)</f>
         <v>25</v>
       </c>
-      <c r="I29" s="94" t="s">
+      <c r="I29" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="122"/>
-      <c r="K29" s="122"/>
+      <c r="J29" s="123"/>
+      <c r="K29" s="123"/>
       <c r="L29" s="69"/>
       <c r="M29" s="69"/>
       <c r="N29" s="69"/>
       <c r="O29" s="69"/>
     </row>
     <row r="30" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="116" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
+      <c r="B30" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="117"/>
       <c r="H30" s="43" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="123" t="e">
+      <c r="J30" s="124" t="e">
         <f aca="false">B29+TIME(0,H30,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K30" s="117" t="str">
+      <c r="K30" s="118" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
@@ -7485,26 +7595,26 @@
       <c r="O30" s="69"/>
     </row>
     <row r="31" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="102" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="102"/>
-      <c r="D31" s="102"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="85" t="n">
+      <c r="B31" s="103" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="86" t="n">
         <v>7</v>
       </c>
-      <c r="I31" s="86" t="s">
+      <c r="I31" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J31" s="124" t="e">
+      <c r="J31" s="125" t="e">
         <f aca="false">J30+TIME(0,H31,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K31" s="104" t="s">
-        <v>110</v>
+      <c r="K31" s="105" t="s">
+        <v>115</v>
       </c>
       <c r="L31" s="69"/>
       <c r="M31" s="69"/>
@@ -7512,25 +7622,25 @@
       <c r="O31" s="69"/>
     </row>
     <row r="32" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="110"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="85" t="n">
+      <c r="B32" s="111" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="111"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="111"/>
+      <c r="H32" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="86" t="s">
+      <c r="I32" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="124" t="e">
+      <c r="J32" s="125" t="e">
         <f aca="false">J31+TIME(0,H32,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K32" s="104" t="str">
+      <c r="K32" s="105" t="str">
         <f aca="false">K30</f>
         <v>{host_name}</v>
       </c>
@@ -7540,26 +7650,26 @@
       <c r="O32" s="69"/>
     </row>
     <row r="33" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="110" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="85" t="n">
+      <c r="B33" s="111" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="111"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="86" t="n">
         <v>7</v>
       </c>
-      <c r="I33" s="86" t="s">
+      <c r="I33" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J33" s="124" t="e">
+      <c r="J33" s="125" t="e">
         <f aca="false">J32+TIME(0,H33,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K33" s="104" t="s">
-        <v>112</v>
+      <c r="K33" s="105" t="s">
+        <v>117</v>
       </c>
       <c r="L33" s="70" t="s">
         <v>59</v>
@@ -7569,25 +7679,25 @@
       <c r="O33" s="70"/>
     </row>
     <row r="34" s="11" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="85" t="n">
+      <c r="B34" s="111" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="111"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="111"/>
+      <c r="F34" s="111"/>
+      <c r="G34" s="111"/>
+      <c r="H34" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="86" t="s">
+      <c r="I34" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="124" t="e">
+      <c r="J34" s="125" t="e">
         <f aca="false">J33+TIME(0,H34,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K34" s="104" t="str">
+      <c r="K34" s="105" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
@@ -7599,26 +7709,26 @@
       <c r="O34" s="71"/>
     </row>
     <row r="35" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="102" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="102"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="102"/>
-      <c r="H35" s="118" t="n">
+      <c r="B35" s="103" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="119" t="n">
         <v>7</v>
       </c>
-      <c r="I35" s="125" t="s">
+      <c r="I35" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="126" t="e">
+      <c r="J35" s="127" t="e">
         <f aca="false">J34+TIME(0,H35,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K35" s="127" t="s">
-        <v>114</v>
+      <c r="K35" s="128" t="s">
+        <v>119</v>
       </c>
       <c r="L35" s="71"/>
       <c r="M35" s="71"/>
@@ -7626,25 +7736,25 @@
       <c r="O35" s="71"/>
     </row>
     <row r="36" s="11" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="119" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="119"/>
-      <c r="D36" s="119"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="119"/>
-      <c r="H36" s="88" t="n">
+      <c r="B36" s="120" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="89" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="89" t="s">
+      <c r="I36" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="128" t="e">
+      <c r="J36" s="129" t="e">
         <f aca="false">J35+TIME(0,H36,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K36" s="90" t="str">
+      <c r="K36" s="91" t="str">
         <f aca="false">K30</f>
         <v>{host_name}</v>
       </c>
@@ -7654,42 +7764,42 @@
       <c r="O36" s="71"/>
     </row>
     <row r="37" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="91" t="e">
+      <c r="B37" s="92" t="e">
         <f aca="false">B29+TIME(0,H29,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C37" s="92" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="93" t="n">
+      <c r="C37" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="93"/>
+      <c r="H37" s="94" t="n">
         <v>5</v>
       </c>
-      <c r="I37" s="94" t="s">
+      <c r="I37" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="95"/>
-      <c r="K37" s="96"/>
+      <c r="J37" s="96"/>
+      <c r="K37" s="97"/>
       <c r="L37" s="71"/>
       <c r="M37" s="71"/>
       <c r="N37" s="71"/>
       <c r="O37" s="71"/>
     </row>
     <row r="38" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="105" t="e">
+      <c r="B38" s="106" t="e">
         <f aca="false">B37+TIME(0,H37,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C38" s="106" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
+      <c r="C38" s="107" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="107"/>
+      <c r="E38" s="107"/>
+      <c r="F38" s="107"/>
+      <c r="G38" s="107"/>
       <c r="H38" s="38" t="n">
         <f aca="false">SUM(H39:H42)</f>
         <v>10</v>
@@ -7705,25 +7815,25 @@
       <c r="O38" s="71"/>
     </row>
     <row r="39" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="116" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="116"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="116"/>
-      <c r="F39" s="116"/>
-      <c r="G39" s="116"/>
+      <c r="B39" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="117"/>
       <c r="H39" s="43" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="123" t="e">
+      <c r="J39" s="124" t="e">
         <f aca="false">B38+TIME(0,H39,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K39" s="117" t="str">
+      <c r="K39" s="118" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
@@ -7733,26 +7843,26 @@
       <c r="O39" s="71"/>
     </row>
     <row r="40" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="102" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="102"/>
-      <c r="D40" s="102"/>
-      <c r="E40" s="102"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="102"/>
-      <c r="H40" s="85" t="n">
+      <c r="B40" s="103" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="103"/>
+      <c r="D40" s="103"/>
+      <c r="E40" s="103"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="86" t="n">
         <v>3</v>
       </c>
-      <c r="I40" s="86" t="s">
+      <c r="I40" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J40" s="124" t="e">
+      <c r="J40" s="125" t="e">
         <f aca="false">J39+TIME(0,H40,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K40" s="104" t="s">
-        <v>98</v>
+      <c r="K40" s="105" t="s">
+        <v>103</v>
       </c>
       <c r="L40" s="71"/>
       <c r="M40" s="71"/>
@@ -7760,26 +7870,26 @@
       <c r="O40" s="71"/>
     </row>
     <row r="41" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="110" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="110"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="110"/>
-      <c r="F41" s="110"/>
-      <c r="G41" s="110"/>
-      <c r="H41" s="85" t="n">
+      <c r="B41" s="111" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="86" t="n">
         <v>3</v>
       </c>
-      <c r="I41" s="86" t="s">
+      <c r="I41" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="124" t="e">
+      <c r="J41" s="125" t="e">
         <f aca="false">J40+TIME(0,H41,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K41" s="104" t="s">
-        <v>119</v>
+      <c r="K41" s="105" t="s">
+        <v>124</v>
       </c>
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
@@ -7787,26 +7897,26 @@
       <c r="O41" s="71"/>
     </row>
     <row r="42" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="102" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="102"/>
-      <c r="D42" s="102"/>
-      <c r="E42" s="102"/>
-      <c r="F42" s="102"/>
-      <c r="G42" s="102"/>
-      <c r="H42" s="85" t="n">
+      <c r="B42" s="103" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="103"/>
+      <c r="D42" s="103"/>
+      <c r="E42" s="103"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="103"/>
+      <c r="H42" s="86" t="n">
         <v>3</v>
       </c>
-      <c r="I42" s="86" t="s">
+      <c r="I42" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J42" s="124" t="e">
+      <c r="J42" s="125" t="e">
         <f aca="false">J41+TIME(0,H42,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K42" s="104" t="s">
-        <v>121</v>
+      <c r="K42" s="105" t="s">
+        <v>126</v>
       </c>
       <c r="L42" s="72" t="s">
         <v>61</v>
@@ -7819,26 +7929,26 @@
       </c>
     </row>
     <row r="43" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="91" t="e">
+      <c r="B43" s="92" t="e">
         <f aca="false">B38+TIME(0,H38,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C43" s="92" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="92"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="92"/>
-      <c r="H43" s="93" t="n">
+      <c r="C43" s="93" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="93"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="93"/>
+      <c r="H43" s="94" t="n">
         <f aca="false">SUM(H44:H48)</f>
         <v>15</v>
       </c>
-      <c r="I43" s="94" t="s">
+      <c r="I43" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
+      <c r="J43" s="94"/>
+      <c r="K43" s="94"/>
       <c r="L43" s="73" t="s">
         <v>62</v>
       </c>
@@ -7850,25 +7960,25 @@
       <c r="P43" s="25"/>
     </row>
     <row r="44" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="129" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="130"/>
-      <c r="D44" s="130"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="130"/>
-      <c r="G44" s="131"/>
-      <c r="H44" s="85" t="n">
+      <c r="B44" s="130" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="131"/>
+      <c r="D44" s="131"/>
+      <c r="E44" s="131"/>
+      <c r="F44" s="131"/>
+      <c r="G44" s="132"/>
+      <c r="H44" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="86" t="s">
+      <c r="I44" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J44" s="32" t="e">
         <f aca="false">B43+TIME(0,H44,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K44" s="100" t="str">
+      <c r="K44" s="101" t="str">
         <f aca="false">K17</f>
         <v>{host_name}</v>
       </c>
@@ -7884,24 +7994,24 @@
     </row>
     <row r="45" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="64" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="64"/>
       <c r="E45" s="64"/>
       <c r="F45" s="64"/>
       <c r="G45" s="64"/>
-      <c r="H45" s="85" t="n">
+      <c r="H45" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="I45" s="86" t="s">
+      <c r="I45" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J45" s="32" t="e">
         <f aca="false">J44+TIME(0,H45,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K45" s="100" t="str">
+      <c r="K45" s="101" t="str">
         <f aca="false">K18</f>
         <v>丘愉庄</v>
       </c>
@@ -7916,24 +8026,24 @@
     </row>
     <row r="46" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="64" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C46" s="64"/>
       <c r="D46" s="64"/>
       <c r="E46" s="64"/>
       <c r="F46" s="64"/>
       <c r="G46" s="64"/>
-      <c r="H46" s="85" t="n">
+      <c r="H46" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="I46" s="86" t="s">
+      <c r="I46" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J46" s="32" t="e">
         <f aca="false">J45+TIME(0,H46,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K46" s="101" t="str">
+      <c r="K46" s="102" t="str">
         <f aca="false">K19</f>
         <v>xxx</v>
       </c>
@@ -7948,24 +8058,24 @@
     </row>
     <row r="47" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="64" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C47" s="64"/>
       <c r="D47" s="64"/>
       <c r="E47" s="64"/>
       <c r="F47" s="64"/>
       <c r="G47" s="64"/>
-      <c r="H47" s="85" t="n">
+      <c r="H47" s="86" t="n">
         <v>3</v>
       </c>
-      <c r="I47" s="86" t="s">
+      <c r="I47" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J47" s="32" t="e">
         <f aca="false">J46+TIME(0,H47,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K47" s="101" t="str">
+      <c r="K47" s="102" t="str">
         <f aca="false">K20</f>
         <v>xxx</v>
       </c>
@@ -7980,25 +8090,25 @@
     </row>
     <row r="48" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="64" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C48" s="64"/>
       <c r="D48" s="64"/>
       <c r="E48" s="64"/>
       <c r="F48" s="64"/>
       <c r="G48" s="64"/>
-      <c r="H48" s="85" t="n">
+      <c r="H48" s="86" t="n">
         <v>7</v>
       </c>
-      <c r="I48" s="86" t="s">
+      <c r="I48" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J48" s="32" t="e">
         <f aca="false">J47+TIME(0,H48,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K48" s="104" t="s">
-        <v>98</v>
+      <c r="K48" s="105" t="s">
+        <v>103</v>
       </c>
       <c r="L48" s="76" t="s">
         <v>72</v>
@@ -8032,26 +8142,26 @@
       <c r="O49" s="81"/>
     </row>
     <row r="50" s="11" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="132" t="e">
+      <c r="B50" s="133" t="e">
         <f aca="false">B43+TIME(0,H43,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C50" s="133" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" s="133"/>
-      <c r="E50" s="133"/>
-      <c r="F50" s="133"/>
-      <c r="G50" s="133"/>
-      <c r="H50" s="134" t="n">
+      <c r="C50" s="134" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="134"/>
+      <c r="E50" s="134"/>
+      <c r="F50" s="134"/>
+      <c r="G50" s="134"/>
+      <c r="H50" s="135" t="n">
         <f aca="false">SUM(H51:H53)</f>
         <v>8</v>
       </c>
-      <c r="I50" s="135" t="s">
+      <c r="I50" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="136"/>
-      <c r="K50" s="122"/>
+      <c r="J50" s="137"/>
+      <c r="K50" s="123"/>
       <c r="L50" s="73" t="s">
         <v>75</v>
       </c>
@@ -8062,26 +8172,26 @@
       <c r="O50" s="75"/>
     </row>
     <row r="51" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="137" t="s">
-        <v>129</v>
-      </c>
-      <c r="C51" s="138"/>
-      <c r="D51" s="138"/>
-      <c r="E51" s="138"/>
-      <c r="F51" s="138"/>
-      <c r="G51" s="139"/>
-      <c r="H51" s="140" t="n">
+      <c r="B51" s="138" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="139"/>
+      <c r="D51" s="139"/>
+      <c r="E51" s="139"/>
+      <c r="F51" s="139"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="141" t="n">
         <v>4</v>
       </c>
-      <c r="I51" s="141" t="s">
+      <c r="I51" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="J51" s="142" t="e">
+      <c r="J51" s="143" t="e">
         <f aca="false">B50+TIME(0,H51,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K51" s="104" t="s">
-        <v>87</v>
+      <c r="K51" s="105" t="s">
+        <v>92</v>
       </c>
       <c r="L51" s="76" t="s">
         <v>77</v>
@@ -8093,21 +8203,21 @@
       <c r="O51" s="78"/>
     </row>
     <row r="52" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="143" t="s">
-        <v>130</v>
-      </c>
-      <c r="H52" s="85" t="n">
+      <c r="B52" s="144" t="s">
+        <v>135</v>
+      </c>
+      <c r="H52" s="86" t="n">
         <v>3</v>
       </c>
-      <c r="I52" s="86" t="s">
+      <c r="I52" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="32" t="e">
         <f aca="false">J51+TIME(0,H52,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K52" s="104" t="s">
-        <v>87</v>
+      <c r="K52" s="105" t="s">
+        <v>92</v>
       </c>
       <c r="L52" s="76" t="s">
         <v>79</v>
@@ -8119,26 +8229,26 @@
       <c r="O52" s="78"/>
     </row>
     <row r="53" s="11" customFormat="true" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="129" t="s">
-        <v>131</v>
-      </c>
-      <c r="C53" s="130"/>
-      <c r="D53" s="130"/>
-      <c r="E53" s="130"/>
-      <c r="F53" s="130"/>
-      <c r="G53" s="131"/>
-      <c r="H53" s="85" t="n">
+      <c r="B53" s="130" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="131"/>
+      <c r="D53" s="131"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="132"/>
+      <c r="H53" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="I53" s="86" t="s">
+      <c r="I53" s="87" t="s">
         <v>22</v>
       </c>
       <c r="J53" s="32" t="e">
         <f aca="false">J52+TIME(0,H53,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K53" s="104" t="s">
-        <v>132</v>
+      <c r="K53" s="105" t="s">
+        <v>137</v>
       </c>
       <c r="L53" s="76" t="s">
         <v>81</v>
@@ -8148,24 +8258,24 @@
         <v>82</v>
       </c>
       <c r="O53" s="78"/>
-      <c r="P53" s="144"/>
+      <c r="P53" s="145"/>
     </row>
     <row r="54" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="132" t="e">
+      <c r="B54" s="133" t="e">
         <f aca="false">B50+TIME(0,H50,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C54" s="133" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="133"/>
-      <c r="E54" s="133"/>
-      <c r="F54" s="133"/>
-      <c r="G54" s="133"/>
-      <c r="H54" s="133"/>
-      <c r="I54" s="145"/>
-      <c r="J54" s="146"/>
-      <c r="K54" s="147"/>
+      <c r="C54" s="134" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="134"/>
+      <c r="E54" s="134"/>
+      <c r="F54" s="134"/>
+      <c r="G54" s="134"/>
+      <c r="H54" s="134"/>
+      <c r="I54" s="146"/>
+      <c r="J54" s="147"/>
+      <c r="K54" s="148"/>
       <c r="L54" s="82" t="s">
         <v>83</v>
       </c>
@@ -8174,7 +8284,7 @@
         <v>84</v>
       </c>
       <c r="O54" s="83"/>
-      <c r="P54" s="144"/>
+      <c r="P54" s="145"/>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add pure text checking
</commit_message>
<xml_diff>
--- a/tm_303_calendar.xlsx
+++ b/tm_303_calendar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" state="visible" r:id="rId2"/>
@@ -2514,7 +2514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2523,252 +2523,28 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+      <left style="hair"/>
       <right/>
-      <top style="medium"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="medium"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium"/>
-      <top style="medium"/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
       <right style="hair"/>
       <top/>
       <bottom/>
@@ -2776,44 +2552,37 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
-      <right style="medium"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+      <left style="hair"/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
+      <right style="hair"/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -2842,7 +2611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2931,87 +2700,83 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="22" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3019,420 +2784,112 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="3" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3522,7 +2979,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>187560</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3537,8 +2994,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894000"/>
-          <a:ext cx="183960" cy="267480"/>
+          <a:off x="4789440" y="15945840"/>
+          <a:ext cx="183960" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3562,7 +3019,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>187560</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3577,8 +3034,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894000"/>
-          <a:ext cx="183960" cy="267480"/>
+          <a:off x="4789440" y="15945840"/>
+          <a:ext cx="183960" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3600,13 +3057,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>59040</xdr:colOff>
+      <xdr:colOff>59400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>271800</xdr:colOff>
+      <xdr:colOff>272160</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
@@ -3621,8 +3078,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="196560" y="195480"/>
-          <a:ext cx="1648440" cy="1323000"/>
+          <a:off x="196920" y="195840"/>
+          <a:ext cx="1648440" cy="1327320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3639,7 +3096,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3654,8 +3111,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5117760"/>
-          <a:ext cx="183960" cy="411840"/>
+          <a:off x="4789440" y="5169600"/>
+          <a:ext cx="183960" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3679,7 +3136,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3694,8 +3151,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5117760"/>
-          <a:ext cx="183960" cy="411840"/>
+          <a:off x="4789440" y="5169600"/>
+          <a:ext cx="183960" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3716,43 +3173,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>97200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>233280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 1032" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5297040" y="11001960"/>
-          <a:ext cx="167040" cy="174600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="9360">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>21</xdr:row>
@@ -3762,16 +3182,16 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>289080</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>293400</xdr:rowOff>
+      <xdr:rowOff>293760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6376320"/>
+          <a:off x="4789440" y="6427800"/>
           <a:ext cx="183960" cy="409320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3802,16 +3222,16 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>289080</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>293400</xdr:rowOff>
+      <xdr:rowOff>293760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6376320"/>
+          <a:off x="4789440" y="6427800"/>
           <a:ext cx="183960" cy="409320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3836,7 +3256,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>188280</xdr:rowOff>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3846,13 +3266,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894720"/>
-          <a:ext cx="183960" cy="267480"/>
+          <a:off x="4789440" y="15946560"/>
+          <a:ext cx="183960" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3876,7 +3296,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>188280</xdr:rowOff>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3886,13 +3306,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894720"/>
-          <a:ext cx="183960" cy="267480"/>
+          <a:off x="4789440" y="15946560"/>
+          <a:ext cx="183960" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3916,7 +3336,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>188280</xdr:rowOff>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3926,13 +3346,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CustomShape 1"/>
+        <xdr:cNvPr id="9" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894720"/>
-          <a:ext cx="183960" cy="267480"/>
+          <a:off x="4789440" y="15946560"/>
+          <a:ext cx="183960" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3956,7 +3376,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>188280</xdr:rowOff>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3966,13 +3386,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
+        <xdr:cNvPr id="10" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="15894720"/>
-          <a:ext cx="183960" cy="267480"/>
+          <a:off x="4789440" y="15946560"/>
+          <a:ext cx="183960" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4002,17 +3422,17 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>289080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>293760</xdr:rowOff>
+      <xdr:rowOff>294120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CustomShape 1"/>
+        <xdr:cNvPr id="11" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5728680"/>
-          <a:ext cx="183960" cy="409320"/>
+          <a:off x="4789440" y="5780160"/>
+          <a:ext cx="183960" cy="409680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4042,7 +3462,47 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>289080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>293760</xdr:rowOff>
+      <xdr:rowOff>294120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4789440" y="5780160"/>
+          <a:ext cx="183960" cy="409680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9360">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>105120</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>188640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>289080</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>294840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4051,8 +3511,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5728680"/>
-          <a:ext cx="183960" cy="409320"/>
+          <a:off x="4789440" y="5474880"/>
+          <a:ext cx="183960" cy="411120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4091,47 +3551,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5423400"/>
-          <a:ext cx="183960" cy="411120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9360">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>105120</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>289080</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>294840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4789440" y="5423400"/>
+          <a:off x="4789440" y="5474880"/>
           <a:ext cx="183960" cy="411120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4156,7 +3576,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>254520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:rowOff>187200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
@@ -4166,17 +3586,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 4" descr=""/>
+        <xdr:cNvPr id="15" name="Picture 4" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12273120" y="348480"/>
-          <a:ext cx="1057320" cy="1193400"/>
+          <a:off x="12273120" y="348840"/>
+          <a:ext cx="1057320" cy="1197720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4193,7 +3613,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -4203,13 +3623,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6032160"/>
-          <a:ext cx="183960" cy="412200"/>
+          <a:off x="4789440" y="6084000"/>
+          <a:ext cx="183960" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4233,7 +3653,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>105120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -4243,13 +3663,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
+        <xdr:cNvPr id="17" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="6032160"/>
-          <a:ext cx="183960" cy="412200"/>
+          <a:off x="4789440" y="6084000"/>
+          <a:ext cx="183960" cy="411840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4279,17 +3699,17 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>289080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>293760</xdr:rowOff>
+      <xdr:rowOff>294120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="CustomShape 1"/>
+        <xdr:cNvPr id="18" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5728680"/>
-          <a:ext cx="183960" cy="409320"/>
+          <a:off x="4789440" y="5780160"/>
+          <a:ext cx="183960" cy="409680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4319,17 +3739,17 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>289080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>293760</xdr:rowOff>
+      <xdr:rowOff>294120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="CustomShape 1"/>
+        <xdr:cNvPr id="19" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789440" y="5728680"/>
-          <a:ext cx="183960" cy="409320"/>
+          <a:off x="4789440" y="5780160"/>
+          <a:ext cx="183960" cy="409680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4351,29 +3771,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>78480</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>193320</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="图片 23" descr=""/>
+        <xdr:cNvPr id="20" name="图片 23" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10987560" y="331560"/>
-          <a:ext cx="1224360" cy="1244160"/>
+          <a:off x="10987920" y="331920"/>
+          <a:ext cx="1224000" cy="1249920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4395,8 +3815,8 @@
   </sheetPr>
   <dimension ref="B2:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4419,7 +3839,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="12.55"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -4455,7 +3875,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="10"/>
     </row>
-    <row r="4" s="11" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
@@ -4473,7 +3893,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="14"/>
     </row>
-    <row r="5" s="11" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="15" t="s">
@@ -4494,7 +3914,7 @@
       <c r="M5" s="13"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="11" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="18" t="s">
         <v>6</v>
       </c>
@@ -4527,1375 +3947,1380 @@
       <c r="O7" s="10"/>
     </row>
     <row r="8" s="11" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="20"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="10"/>
-    </row>
-    <row r="9" s="23" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="24" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="27"/>
+    </row>
+    <row r="9" s="28" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26" t="s">
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
     </row>
     <row r="10" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
     </row>
     <row r="11" s="11" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="29"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="35" t="s">
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="32" t="s">
+      <c r="K11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
     </row>
     <row r="12" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="40"/>
+      <c r="J12" s="41"/>
       <c r="K12" s="41"/>
-      <c r="L12" s="42" t="s">
+      <c r="L12" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-    </row>
-    <row r="13" s="43" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="44" t="s">
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+    </row>
+    <row r="13" s="42" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="45" t="s">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="46" t="s">
+      <c r="I13" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="48" t="s">
+      <c r="K13" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="49" t="s">
+      <c r="L13" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="50" t="s">
+      <c r="M13" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="51" t="s">
+      <c r="N13" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="52" t="s">
+      <c r="O13" s="49" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" s="43" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="53" t="s">
+    <row r="14" s="42" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="54" t="n">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="31" t="e">
+      <c r="J14" s="34" t="e">
         <f aca="false">J13+TIME(0,H14,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="56" t="s">
+      <c r="L14" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="57" t="s">
+      <c r="M14" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="57" t="s">
+      <c r="N14" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="O14" s="58" t="s">
+      <c r="O14" s="50" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" s="43" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="59" t="s">
+    <row r="15" s="42" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60" t="n">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="61" t="s">
+      <c r="I15" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="35" t="e">
+      <c r="J15" s="34" t="e">
         <f aca="false">J14+TIME(0,H15,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K15" s="62" t="s">
+      <c r="K15" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="63" t="s">
+      <c r="L15" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="64" t="s">
+      <c r="M15" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="N15" s="64" t="s">
+      <c r="N15" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="65" t="s">
+      <c r="O15" s="50" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" s="43" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="66" t="e">
+    <row r="16" s="42" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="38" t="e">
         <f aca="false">B12+TIME(0,H12,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68" t="n">
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="39" t="n">
         <f aca="false">SUM(H17:H21)</f>
         <v>9</v>
       </c>
-      <c r="I16" s="69" t="s">
+      <c r="I16" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="70"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="72" t="s">
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
     </row>
     <row r="17" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="74" t="n">
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="55" t="s">
+      <c r="I17" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="31" t="e">
+      <c r="J17" s="34" t="e">
         <f aca="false">B16+TIME(0,H17,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K17" s="75" t="str">
+      <c r="K17" s="43" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
-      <c r="L17" s="44" t="s">
+      <c r="L17" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="M17" s="30" t="s">
+      <c r="M17" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="76" t="n">
+      <c r="N17" s="43" t="n">
         <v>13826106387</v>
       </c>
-      <c r="O17" s="76"/>
+      <c r="O17" s="43"/>
     </row>
     <row r="18" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="54" t="n">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="55" t="s">
+      <c r="I18" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="31" t="e">
+      <c r="J18" s="34" t="e">
         <f aca="false">J17+TIME(0,H18,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K18" s="77" t="s">
+      <c r="K18" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="53" t="s">
+      <c r="L18" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="30" t="s">
+      <c r="M18" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="N18" s="76" t="n">
+      <c r="N18" s="43" t="n">
         <v>13794874425</v>
       </c>
-      <c r="O18" s="76"/>
+      <c r="O18" s="43"/>
     </row>
     <row r="19" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="54" t="n">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="55" t="s">
+      <c r="I19" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="31" t="e">
+      <c r="J19" s="34" t="e">
         <f aca="false">J18+TIME(0,H19,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K19" s="78" t="s">
+      <c r="K19" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="L19" s="53" t="s">
+      <c r="L19" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="M19" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="N19" s="76" t="n">
+      <c r="N19" s="43" t="n">
         <v>13533880814</v>
       </c>
-      <c r="O19" s="76"/>
+      <c r="O19" s="43"/>
     </row>
     <row r="20" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="54" t="n">
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I20" s="55" t="s">
+      <c r="I20" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="31" t="e">
+      <c r="J20" s="34" t="e">
         <f aca="false">J19+TIME(0,H20,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K20" s="78" t="s">
+      <c r="K20" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="53" t="s">
+      <c r="L20" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="76" t="n">
+      <c r="N20" s="43" t="n">
         <v>15920428594</v>
       </c>
-      <c r="O20" s="76"/>
+      <c r="O20" s="43"/>
     </row>
     <row r="21" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="54" t="n">
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I21" s="55" t="s">
+      <c r="I21" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="31" t="e">
+      <c r="J21" s="34" t="e">
         <f aca="false">J20+TIME(0,H21,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K21" s="81" t="s">
+      <c r="K21" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L21" s="53" t="s">
+      <c r="L21" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="M21" s="30" t="s">
+      <c r="M21" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="76" t="n">
+      <c r="N21" s="43" t="n">
         <v>18028652848</v>
       </c>
-      <c r="O21" s="76"/>
+      <c r="O21" s="43"/>
     </row>
     <row r="22" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="54" t="n">
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="31" t="e">
+      <c r="J22" s="34" t="e">
         <f aca="false">J21+TIME(0,H22,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K22" s="77" t="s">
+      <c r="K22" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="L22" s="53" t="s">
+      <c r="L22" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="30" t="s">
+      <c r="M22" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="76" t="n">
+      <c r="N22" s="43" t="n">
         <v>13022004144</v>
       </c>
-      <c r="O22" s="76"/>
+      <c r="O22" s="43"/>
     </row>
     <row r="23" s="11" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="82" t="e">
+      <c r="B23" s="38" t="e">
         <f aca="false">B16+TIME(0,H16,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C23" s="83" t="s">
+      <c r="C23" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="84" t="n">
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="39" t="n">
         <f aca="false">SUM(H24:H28)</f>
         <v>29</v>
       </c>
-      <c r="I23" s="85" t="s">
+      <c r="I23" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="53" t="s">
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="76" t="n">
+      <c r="N23" s="43" t="n">
         <v>18127871902</v>
       </c>
-      <c r="O23" s="76"/>
+      <c r="O23" s="43"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="54" t="n">
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="55" t="s">
+      <c r="I24" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="31" t="e">
+      <c r="J24" s="34" t="e">
         <f aca="false">B23+TIME(0,H24,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K24" s="88" t="s">
+      <c r="K24" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="L24" s="89" t="s">
+      <c r="L24" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="M24" s="90" t="s">
+      <c r="M24" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="91" t="n">
+      <c r="N24" s="43" t="n">
         <v>18688883546</v>
       </c>
-      <c r="O24" s="91"/>
+      <c r="O24" s="43"/>
     </row>
     <row r="25" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="93" t="n">
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I25" s="94" t="s">
+      <c r="I25" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="95" t="e">
+      <c r="J25" s="34" t="e">
         <f aca="false">J24+TIME(0,H25,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K25" s="62" t="s">
+      <c r="K25" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="L25" s="96" t="s">
+      <c r="L25" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="M25" s="96"/>
-      <c r="N25" s="96"/>
-      <c r="O25" s="96"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="45" t="n">
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="43" t="n">
         <v>18</v>
       </c>
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="47" t="e">
+      <c r="J26" s="34" t="e">
         <f aca="false">J25+TIME(0,H26,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K26" s="98" t="s">
+      <c r="K26" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="L26" s="99" t="s">
+      <c r="L26" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="M26" s="99"/>
-      <c r="N26" s="99"/>
-      <c r="O26" s="99"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
     </row>
     <row r="27" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="100" t="n">
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="I27" s="55" t="s">
+      <c r="I27" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="31" t="e">
+      <c r="J27" s="34" t="e">
         <f aca="false">J26+TIME(0,H27,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K27" s="81" t="s">
+      <c r="K27" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="L27" s="99"/>
-      <c r="M27" s="99"/>
-      <c r="N27" s="99"/>
-      <c r="O27" s="99"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="102" t="n">
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="61" t="s">
+      <c r="I28" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="35" t="e">
+      <c r="J28" s="34" t="e">
         <f aca="false">J27+TIME(0,H28,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K28" s="103" t="str">
+      <c r="K28" s="58" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
-      <c r="L28" s="99"/>
-      <c r="M28" s="99"/>
-      <c r="N28" s="99"/>
-      <c r="O28" s="99"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
     </row>
     <row r="29" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="66" t="e">
+      <c r="B29" s="38" t="e">
         <f aca="false">B23+TIME(0,H23,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="68" t="n">
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="39" t="n">
         <f aca="false">SUM(H30:H36)</f>
         <v>25</v>
       </c>
-      <c r="I29" s="69" t="s">
+      <c r="I29" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="104"/>
-      <c r="K29" s="104"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="99"/>
-      <c r="N29" s="99"/>
-      <c r="O29" s="99"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
     </row>
     <row r="30" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="97"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="97"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="45" t="n">
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I30" s="46" t="s">
+      <c r="I30" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="105" t="e">
+      <c r="J30" s="59" t="e">
         <f aca="false">B29+TIME(0,H30,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K30" s="98" t="str">
+      <c r="K30" s="51" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
-      <c r="L30" s="99"/>
-      <c r="M30" s="99"/>
-      <c r="N30" s="99"/>
-      <c r="O30" s="99"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
     </row>
     <row r="31" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="54" t="n">
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="I31" s="55" t="s">
+      <c r="I31" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J31" s="106" t="e">
+      <c r="J31" s="59" t="e">
         <f aca="false">J30+TIME(0,H31,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K31" s="81" t="s">
+      <c r="K31" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="99"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="99"/>
-      <c r="O31" s="99"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
     </row>
     <row r="32" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="87" t="s">
+      <c r="B32" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="54" t="n">
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="55" t="s">
+      <c r="I32" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="106" t="e">
+      <c r="J32" s="59" t="e">
         <f aca="false">J31+TIME(0,H32,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K32" s="81" t="str">
+      <c r="K32" s="51" t="str">
         <f aca="false">K30</f>
         <v>{host_name}</v>
       </c>
-      <c r="L32" s="99"/>
-      <c r="M32" s="99"/>
-      <c r="N32" s="99"/>
-      <c r="O32" s="99"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
     </row>
     <row r="33" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="54" t="n">
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="I33" s="55" t="s">
+      <c r="I33" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="106" t="e">
+      <c r="J33" s="59" t="e">
         <f aca="false">J32+TIME(0,H33,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K33" s="81" t="s">
+      <c r="K33" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="L33" s="107" t="s">
+      <c r="L33" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="M33" s="107"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="55"/>
     </row>
     <row r="34" s="11" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="87" t="s">
+      <c r="B34" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="54" t="n">
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="55" t="s">
+      <c r="I34" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J34" s="106" t="e">
+      <c r="J34" s="59" t="e">
         <f aca="false">J33+TIME(0,H34,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K34" s="81" t="str">
+      <c r="K34" s="51" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
-      <c r="L34" s="108" t="s">
+      <c r="L34" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="M34" s="108"/>
-      <c r="N34" s="108"/>
-      <c r="O34" s="108"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
     </row>
     <row r="35" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="100" t="n">
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="I35" s="109" t="s">
+      <c r="I35" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="J35" s="110" t="e">
+      <c r="J35" s="62" t="e">
         <f aca="false">J34+TIME(0,H35,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K35" s="111" t="s">
+      <c r="K35" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="L35" s="108"/>
-      <c r="M35" s="108"/>
-      <c r="N35" s="108"/>
-      <c r="O35" s="108"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
     </row>
     <row r="36" s="11" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="101" t="s">
+      <c r="B36" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="101"/>
-      <c r="D36" s="101"/>
-      <c r="E36" s="101"/>
-      <c r="F36" s="101"/>
-      <c r="G36" s="101"/>
-      <c r="H36" s="60" t="n">
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="61" t="s">
+      <c r="I36" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J36" s="112" t="e">
+      <c r="J36" s="59" t="e">
         <f aca="false">J35+TIME(0,H36,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K36" s="62" t="str">
+      <c r="K36" s="51" t="str">
         <f aca="false">K30</f>
         <v>{host_name}</v>
       </c>
-      <c r="L36" s="108"/>
-      <c r="M36" s="108"/>
-      <c r="N36" s="108"/>
-      <c r="O36" s="108"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
     </row>
     <row r="37" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="66" t="e">
+      <c r="B37" s="38" t="e">
         <f aca="false">B29+TIME(0,H29,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="68" t="n">
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="39" t="n">
         <v>5</v>
       </c>
-      <c r="I37" s="69" t="s">
+      <c r="I37" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="70"/>
-      <c r="K37" s="71"/>
-      <c r="L37" s="108"/>
-      <c r="M37" s="108"/>
-      <c r="N37" s="108"/>
-      <c r="O37" s="108"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
     </row>
     <row r="38" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="82" t="e">
+      <c r="B38" s="38" t="e">
         <f aca="false">B37+TIME(0,H37,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C38" s="83" t="s">
+      <c r="C38" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="38" t="n">
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="39" t="n">
         <f aca="false">SUM(H39:H42)</f>
         <v>10</v>
       </c>
-      <c r="I38" s="39" t="s">
+      <c r="I38" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="108"/>
-      <c r="M38" s="108"/>
-      <c r="N38" s="108"/>
-      <c r="O38" s="108"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
     </row>
     <row r="39" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="97" t="s">
+      <c r="B39" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="97"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="97"/>
-      <c r="G39" s="97"/>
-      <c r="H39" s="45" t="n">
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I39" s="46" t="s">
+      <c r="I39" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="105" t="e">
+      <c r="J39" s="59" t="e">
         <f aca="false">B38+TIME(0,H39,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K39" s="98" t="str">
+      <c r="K39" s="51" t="str">
         <f aca="false">K13</f>
         <v>{host_name}</v>
       </c>
-      <c r="L39" s="108"/>
-      <c r="M39" s="108"/>
-      <c r="N39" s="108"/>
-      <c r="O39" s="108"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="60"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
     </row>
     <row r="40" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="79"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="54" t="n">
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="I40" s="55" t="s">
+      <c r="I40" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J40" s="106" t="e">
+      <c r="J40" s="59" t="e">
         <f aca="false">J39+TIME(0,H40,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K40" s="81" t="s">
+      <c r="K40" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="108"/>
-      <c r="M40" s="108"/>
-      <c r="N40" s="108"/>
-      <c r="O40" s="108"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
     </row>
     <row r="41" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="87" t="s">
+      <c r="B41" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="87"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="54" t="n">
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="I41" s="55" t="s">
+      <c r="I41" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="106" t="e">
+      <c r="J41" s="59" t="e">
         <f aca="false">J40+TIME(0,H41,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K41" s="81" t="s">
+      <c r="K41" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="L41" s="108"/>
-      <c r="M41" s="108"/>
-      <c r="N41" s="108"/>
-      <c r="O41" s="108"/>
+      <c r="L41" s="60"/>
+      <c r="M41" s="60"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="60"/>
     </row>
     <row r="42" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="79" t="s">
+      <c r="B42" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="79"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="79"/>
-      <c r="G42" s="79"/>
-      <c r="H42" s="54" t="n">
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="I42" s="55" t="s">
+      <c r="I42" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="106" t="e">
+      <c r="J42" s="59" t="e">
         <f aca="false">J41+TIME(0,H42,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K42" s="81" t="s">
+      <c r="K42" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="L42" s="113" t="s">
+      <c r="L42" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="M42" s="113"/>
-      <c r="N42" s="113"/>
-      <c r="O42" s="113"/>
-      <c r="P42" s="114" t="s">
+      <c r="M42" s="55"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="63" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="66" t="e">
+      <c r="B43" s="38" t="e">
         <f aca="false">B38+TIME(0,H38,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C43" s="67" t="s">
+      <c r="C43" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
-      <c r="H43" s="68" t="n">
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="39" t="n">
         <f aca="false">SUM(H44:H48)</f>
         <v>15</v>
       </c>
-      <c r="I43" s="69" t="s">
+      <c r="I43" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="115" t="s">
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116" t="s">
+      <c r="M43" s="64"/>
+      <c r="N43" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="O43" s="117"/>
-      <c r="P43" s="114"/>
+      <c r="O43" s="64"/>
+      <c r="P43" s="63"/>
     </row>
     <row r="44" s="11" customFormat="true" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="118" t="s">
+      <c r="B44" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="119"/>
-      <c r="D44" s="119"/>
-      <c r="E44" s="119"/>
-      <c r="F44" s="119"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="54" t="n">
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="55" t="s">
+      <c r="I44" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J44" s="31" t="e">
+      <c r="J44" s="34" t="e">
         <f aca="false">B43+TIME(0,H44,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K44" s="77" t="str">
+      <c r="K44" s="51" t="str">
         <f aca="false">K17</f>
         <v>{host_name}</v>
       </c>
-      <c r="L44" s="121" t="s">
+      <c r="L44" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="M44" s="122"/>
-      <c r="N44" s="122" t="s">
+      <c r="M44" s="64"/>
+      <c r="N44" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="O44" s="123"/>
-      <c r="P44" s="114"/>
+      <c r="O44" s="64"/>
+      <c r="P44" s="63"/>
     </row>
     <row r="45" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="54" t="n">
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I45" s="55" t="s">
+      <c r="I45" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="31" t="e">
+      <c r="J45" s="34" t="e">
         <f aca="false">J44+TIME(0,H45,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K45" s="77" t="str">
+      <c r="K45" s="51" t="str">
         <f aca="false">K18</f>
         <v>丘愉庄</v>
       </c>
-      <c r="L45" s="121" t="s">
+      <c r="L45" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="M45" s="122"/>
-      <c r="N45" s="122" t="s">
+      <c r="M45" s="64"/>
+      <c r="N45" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="O45" s="123"/>
+      <c r="O45" s="64"/>
     </row>
     <row r="46" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="54" t="n">
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I46" s="55" t="s">
+      <c r="I46" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J46" s="31" t="e">
+      <c r="J46" s="34" t="e">
         <f aca="false">J45+TIME(0,H46,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K46" s="78" t="str">
+      <c r="K46" s="52" t="str">
         <f aca="false">K19</f>
         <v>xxx</v>
       </c>
-      <c r="L46" s="121" t="s">
+      <c r="L46" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="M46" s="122"/>
-      <c r="N46" s="122" t="s">
+      <c r="M46" s="64"/>
+      <c r="N46" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="O46" s="123"/>
+      <c r="O46" s="64"/>
     </row>
     <row r="47" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="54" t="n">
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="I47" s="55" t="s">
+      <c r="I47" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J47" s="31" t="e">
+      <c r="J47" s="34" t="e">
         <f aca="false">J46+TIME(0,H47,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K47" s="78" t="str">
+      <c r="K47" s="52" t="str">
         <f aca="false">K20</f>
         <v>xxx</v>
       </c>
-      <c r="L47" s="121" t="s">
+      <c r="L47" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="M47" s="122"/>
-      <c r="N47" s="122" t="s">
+      <c r="M47" s="64"/>
+      <c r="N47" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="O47" s="123"/>
+      <c r="O47" s="64"/>
     </row>
     <row r="48" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="54" t="n">
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="I48" s="55" t="s">
+      <c r="I48" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J48" s="31" t="e">
+      <c r="J48" s="34" t="e">
         <f aca="false">J47+TIME(0,H48,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K48" s="81" t="s">
+      <c r="K48" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L48" s="121" t="s">
+      <c r="L48" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="M48" s="122"/>
-      <c r="N48" s="124"/>
-      <c r="O48" s="124"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="65"/>
+      <c r="O48" s="65"/>
     </row>
     <row r="49" s="11" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="125" t="s">
+      <c r="B49" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="C49" s="125" t="s">
+      <c r="C49" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="126"/>
-      <c r="E49" s="126"/>
-      <c r="F49" s="126"/>
-      <c r="G49" s="126"/>
-      <c r="H49" s="126"/>
-      <c r="I49" s="126"/>
-      <c r="J49" s="126"/>
-      <c r="K49" s="127"/>
-      <c r="L49" s="128" t="s">
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="M49" s="128"/>
-      <c r="N49" s="129" t="s">
+      <c r="M49" s="31"/>
+      <c r="N49" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="O49" s="129"/>
+      <c r="O49" s="31"/>
     </row>
     <row r="50" s="11" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="130" t="e">
+      <c r="B50" s="38" t="e">
         <f aca="false">B43+TIME(0,H43,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C50" s="131" t="s">
+      <c r="C50" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D50" s="131"/>
-      <c r="E50" s="131"/>
-      <c r="F50" s="131"/>
-      <c r="G50" s="131"/>
-      <c r="H50" s="132" t="n">
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="39" t="n">
         <f aca="false">SUM(H51:H53)</f>
         <v>8</v>
       </c>
-      <c r="I50" s="133" t="s">
+      <c r="I50" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J50" s="134"/>
-      <c r="K50" s="104"/>
-      <c r="L50" s="115" t="s">
+      <c r="J50" s="41"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="M50" s="115"/>
-      <c r="N50" s="117" t="s">
+      <c r="M50" s="64"/>
+      <c r="N50" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="O50" s="117"/>
+      <c r="O50" s="64"/>
     </row>
     <row r="51" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="135" t="s">
+      <c r="B51" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="C51" s="136"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136"/>
-      <c r="F51" s="136"/>
-      <c r="G51" s="137"/>
-      <c r="H51" s="138" t="n">
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="57" t="n">
         <v>4</v>
       </c>
-      <c r="I51" s="139" t="s">
+      <c r="I51" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="J51" s="140" t="e">
+      <c r="J51" s="67" t="e">
         <f aca="false">B50+TIME(0,H51,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K51" s="81" t="s">
+      <c r="K51" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="L51" s="121" t="s">
+      <c r="L51" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="M51" s="121"/>
-      <c r="N51" s="123" t="s">
+      <c r="M51" s="64"/>
+      <c r="N51" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="O51" s="123"/>
+      <c r="O51" s="64"/>
     </row>
     <row r="52" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="141" t="s">
+      <c r="B52" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="H52" s="54" t="n">
+      <c r="C52" s="68"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="I52" s="55" t="s">
+      <c r="I52" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J52" s="31" t="e">
+      <c r="J52" s="34" t="e">
         <f aca="false">J51+TIME(0,H52,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K52" s="81" t="s">
+      <c r="K52" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="L52" s="121" t="s">
+      <c r="L52" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="M52" s="121"/>
-      <c r="N52" s="123" t="s">
+      <c r="M52" s="64"/>
+      <c r="N52" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="O52" s="123"/>
+      <c r="O52" s="64"/>
     </row>
     <row r="53" s="11" customFormat="true" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="118" t="s">
+      <c r="B53" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="119"/>
-      <c r="D53" s="119"/>
-      <c r="E53" s="119"/>
-      <c r="F53" s="119"/>
-      <c r="G53" s="120"/>
-      <c r="H53" s="54" t="n">
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I53" s="55" t="s">
+      <c r="I53" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J53" s="31" t="e">
+      <c r="J53" s="34" t="e">
         <f aca="false">J52+TIME(0,H53,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K53" s="81" t="s">
+      <c r="K53" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="L53" s="121" t="s">
+      <c r="L53" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="M53" s="121"/>
-      <c r="N53" s="123" t="s">
+      <c r="M53" s="64"/>
+      <c r="N53" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="O53" s="123"/>
-      <c r="P53" s="142"/>
+      <c r="O53" s="64"/>
+      <c r="P53" s="69"/>
     </row>
     <row r="54" s="11" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="130" t="e">
+      <c r="B54" s="38" t="e">
         <f aca="false">B50+TIME(0,H50,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C54" s="131" t="s">
+      <c r="C54" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="D54" s="131"/>
-      <c r="E54" s="131"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="131"/>
-      <c r="I54" s="143"/>
-      <c r="J54" s="144"/>
-      <c r="K54" s="145"/>
-      <c r="L54" s="146" t="s">
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="M54" s="146"/>
-      <c r="N54" s="147" t="s">
+      <c r="M54" s="64"/>
+      <c r="N54" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="O54" s="147"/>
-      <c r="P54" s="142"/>
+      <c r="O54" s="64"/>
+      <c r="P54" s="69"/>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5910,7 +5335,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="81">
     <mergeCell ref="B2:C5"/>
     <mergeCell ref="E2:N2"/>
     <mergeCell ref="E3:N3"/>
@@ -5970,11 +5395,13 @@
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="L42:O42"/>
     <mergeCell ref="C43:G43"/>
+    <mergeCell ref="B44:G44"/>
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="B46:G46"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="N48:O48"/>
+    <mergeCell ref="C49:K49"/>
     <mergeCell ref="L49:M49"/>
     <mergeCell ref="N49:O49"/>
     <mergeCell ref="C50:G50"/>
@@ -5987,7 +5414,7 @@
     <mergeCell ref="L53:M53"/>
     <mergeCell ref="N53:O53"/>
     <mergeCell ref="P53:P55"/>
-    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C54:K54"/>
     <mergeCell ref="L54:M54"/>
     <mergeCell ref="N54:O54"/>
   </mergeCells>
@@ -6009,7 +5436,7 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6019,112 +5446,112 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="71" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="71" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="149" t="s">
+      <c r="A3" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="71" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="71" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="149" t="s">
+      <c r="C5" s="71" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="149" t="s">
+      <c r="A6" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="149" t="s">
+      <c r="B6" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="149" t="s">
+      <c r="C6" s="71" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="149" t="s">
+      <c r="A7" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="149" t="s">
+      <c r="B7" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="149" t="s">
+      <c r="C7" s="71" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="149" t="s">
+      <c r="A8" s="71" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="149" t="s">
+      <c r="B8" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="149" t="s">
+      <c r="C8" s="71" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="149" t="s">
+      <c r="A9" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="149" t="s">
+      <c r="B9" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="149" t="s">
+      <c r="C9" s="71" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="149" t="s">
+      <c r="C10" s="71" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>